<commit_message>
Update Business intelligence systems - Project - Loan Portfolio Data Specification - V6.3.xlsx
</commit_message>
<xml_diff>
--- a/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.3.xlsx
+++ b/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ShrForms\specifications\lp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493D002D-5AE7-40E1-B111-700776D32D6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC310A1-CE8C-42B2-AE86-A28DBC079F58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="804" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2705" uniqueCount="1616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2708" uniqueCount="1619">
   <si>
     <t>Field ID</t>
   </si>
@@ -5259,6 +5259,15 @@
     <t>A nil Return can only be entered if:
 1. No in-year return exists for that financial year;
 2. No live Facility or ISDA or Inter Group Finance record exists in the previous annual return;</t>
+  </si>
+  <si>
+    <t>LPL101</t>
+  </si>
+  <si>
+    <t>Loan Covenants</t>
+  </si>
+  <si>
+    <t>Select({"page":"loancovenant", "createLabel":"Add existing Loan Covenant", "title":"Select Loan Covenants", "useParent": true, "columns":["lpc004"]})</t>
   </si>
 </sst>
 </file>
@@ -6378,19 +6387,19 @@
     <xf numFmtId="0" fontId="32" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7308,7 +7317,7 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="Data!H172">
+    <xdr:sp macro="" textlink="Data!H173">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
@@ -8674,15 +8683,15 @@
     </row>
     <row r="73" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="80">
-        <f>Data!I170</f>
+        <f>Data!I171</f>
         <v>1</v>
       </c>
       <c r="C73" s="147" t="str">
-        <f>Data!H171</f>
+        <f>Data!H172</f>
         <v>Debt Service Test (DST)</v>
       </c>
       <c r="D73" s="198" t="str">
-        <f>Data!H174</f>
+        <f>Data!H175</f>
         <v>Monthly</v>
       </c>
       <c r="E73" s="198"/>
@@ -8717,19 +8726,19 @@
     </row>
     <row r="78" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="80">
-        <f>Data!I180</f>
+        <f>Data!I181</f>
         <v>1</v>
       </c>
       <c r="C78" s="147" t="str">
-        <f>Data!H181</f>
+        <f>Data!H182</f>
         <v>Embedded interest rate swap</v>
       </c>
       <c r="D78" s="148">
-        <f>Data!H183</f>
+        <f>Data!H184</f>
         <v>38443</v>
       </c>
       <c r="E78" s="148">
-        <f>Data!H184</f>
+        <f>Data!H185</f>
         <v>42094</v>
       </c>
       <c r="F78" s="153" t="s">
@@ -8781,7 +8790,7 @@
         <v>1533</v>
       </c>
       <c r="B3" s="140">
-        <f>Data!I168</f>
+        <f>Data!I169</f>
         <v>1</v>
       </c>
     </row>
@@ -8790,7 +8799,7 @@
         <v>1520</v>
       </c>
       <c r="B5" s="140" t="str">
-        <f>Data!I169</f>
+        <f>Data!I170</f>
         <v>BOSFIXED0001</v>
       </c>
     </row>
@@ -8799,7 +8808,7 @@
         <v>1342</v>
       </c>
       <c r="B7" s="140">
-        <f>Data!I170</f>
+        <f>Data!I171</f>
         <v>1</v>
       </c>
     </row>
@@ -8808,7 +8817,7 @@
         <v>345</v>
       </c>
       <c r="B9" t="str">
-        <f>Data!H171</f>
+        <f>Data!H172</f>
         <v>Debt Service Test (DST)</v>
       </c>
     </row>
@@ -8822,7 +8831,7 @@
         <v>346</v>
       </c>
       <c r="B18" t="str">
-        <f>Data!H173</f>
+        <f>Data!H174</f>
         <v>105%</v>
       </c>
     </row>
@@ -8831,7 +8840,7 @@
         <v>347</v>
       </c>
       <c r="B20" t="str">
-        <f>Data!H174</f>
+        <f>Data!H175</f>
         <v>Monthly</v>
       </c>
     </row>
@@ -8840,7 +8849,7 @@
         <v>348</v>
       </c>
       <c r="B22" s="112">
-        <f>Data!H175</f>
+        <f>Data!H176</f>
         <v>40269</v>
       </c>
     </row>
@@ -8849,7 +8858,7 @@
         <v>349</v>
       </c>
       <c r="B24" t="str">
-        <f>Data!H176</f>
+        <f>Data!H177</f>
         <v>115%</v>
       </c>
     </row>
@@ -8885,7 +8894,7 @@
         <v>1533</v>
       </c>
       <c r="B3" s="140">
-        <f>Data!I178</f>
+        <f>Data!I179</f>
         <v>1</v>
       </c>
     </row>
@@ -8894,7 +8903,7 @@
         <v>1520</v>
       </c>
       <c r="B5" s="140" t="str">
-        <f>Data!I179</f>
+        <f>Data!I180</f>
         <v>BOSFIXED0001</v>
       </c>
     </row>
@@ -8903,7 +8912,7 @@
         <v>1342</v>
       </c>
       <c r="B7" s="140">
-        <f>Data!I180</f>
+        <f>Data!I181</f>
         <v>1</v>
       </c>
     </row>
@@ -8912,7 +8921,7 @@
         <v>1534</v>
       </c>
       <c r="B9" t="str">
-        <f>Data!H181</f>
+        <f>Data!H182</f>
         <v>Embedded interest rate swap</v>
       </c>
     </row>
@@ -8921,7 +8930,7 @@
         <v>178</v>
       </c>
       <c r="B11">
-        <f>Data!H182</f>
+        <f>Data!H183</f>
         <v>5000</v>
       </c>
     </row>
@@ -8933,7 +8942,7 @@
         <v>1535</v>
       </c>
       <c r="B13" s="112">
-        <f>Data!H183</f>
+        <f>Data!H184</f>
         <v>38443</v>
       </c>
     </row>
@@ -8942,7 +8951,7 @@
         <v>1536</v>
       </c>
       <c r="B15" s="112">
-        <f>Data!H184</f>
+        <f>Data!H185</f>
         <v>42094</v>
       </c>
     </row>
@@ -8951,7 +8960,7 @@
         <v>1537</v>
       </c>
       <c r="B17">
-        <f>Data!H185</f>
+        <f>Data!H186</f>
         <v>20.0001</v>
       </c>
     </row>
@@ -8960,7 +8969,7 @@
         <v>1538</v>
       </c>
       <c r="B19">
-        <f>Data!H186</f>
+        <f>Data!H187</f>
         <v>3.875</v>
       </c>
     </row>
@@ -8969,7 +8978,7 @@
         <v>1539</v>
       </c>
       <c r="B21" t="b">
-        <f>Data!H187</f>
+        <f>Data!H188</f>
         <v>1</v>
       </c>
     </row>
@@ -9093,12 +9102,12 @@
       <c r="D8" s="199" t="s">
         <v>177</v>
       </c>
-      <c r="E8" s="202"/>
-      <c r="F8" s="200"/>
+      <c r="E8" s="200"/>
+      <c r="F8" s="201"/>
       <c r="G8" s="199" t="s">
         <v>178</v>
       </c>
-      <c r="H8" s="200"/>
+      <c r="H8" s="201"/>
       <c r="I8" s="75"/>
       <c r="J8" s="75"/>
     </row>
@@ -9106,15 +9115,15 @@
       <c r="C9" s="76">
         <v>1431</v>
       </c>
-      <c r="D9" s="203" t="s">
+      <c r="D9" s="202" t="s">
         <v>458</v>
       </c>
-      <c r="E9" s="203"/>
-      <c r="F9" s="203"/>
-      <c r="G9" s="201">
+      <c r="E9" s="202"/>
+      <c r="F9" s="202"/>
+      <c r="G9" s="204">
         <v>1000.1</v>
       </c>
-      <c r="H9" s="201"/>
+      <c r="H9" s="204"/>
       <c r="I9" s="79" t="s">
         <v>1131</v>
       </c>
@@ -9126,15 +9135,15 @@
       <c r="C10" s="76">
         <v>1432</v>
       </c>
-      <c r="D10" s="203" t="s">
+      <c r="D10" s="202" t="s">
         <v>467</v>
       </c>
-      <c r="E10" s="203"/>
-      <c r="F10" s="203"/>
-      <c r="G10" s="201">
+      <c r="E10" s="202"/>
+      <c r="F10" s="202"/>
+      <c r="G10" s="204">
         <v>2000.9</v>
       </c>
-      <c r="H10" s="201"/>
+      <c r="H10" s="204"/>
       <c r="I10" s="79" t="s">
         <v>1131</v>
       </c>
@@ -9159,12 +9168,12 @@
       <c r="D12" s="199" t="s">
         <v>345</v>
       </c>
-      <c r="E12" s="200"/>
+      <c r="E12" s="201"/>
       <c r="F12" s="199" t="s">
         <v>347</v>
       </c>
-      <c r="G12" s="202"/>
-      <c r="H12" s="200"/>
+      <c r="G12" s="200"/>
+      <c r="H12" s="201"/>
       <c r="I12" s="75"/>
       <c r="J12" s="75"/>
     </row>
@@ -9172,15 +9181,15 @@
       <c r="C13" s="76">
         <v>13475</v>
       </c>
-      <c r="D13" s="203" t="s">
+      <c r="D13" s="202" t="s">
         <v>909</v>
       </c>
-      <c r="E13" s="203"/>
-      <c r="F13" s="203" t="s">
+      <c r="E13" s="202"/>
+      <c r="F13" s="202" t="s">
         <v>888</v>
       </c>
-      <c r="G13" s="203"/>
-      <c r="H13" s="203"/>
+      <c r="G13" s="202"/>
+      <c r="H13" s="202"/>
       <c r="I13" s="79" t="s">
         <v>1131</v>
       </c>
@@ -9192,15 +9201,15 @@
       <c r="C14" s="76">
         <v>13476</v>
       </c>
-      <c r="D14" s="203" t="s">
+      <c r="D14" s="202" t="s">
         <v>927</v>
       </c>
-      <c r="E14" s="203"/>
-      <c r="F14" s="203" t="s">
+      <c r="E14" s="202"/>
+      <c r="F14" s="202" t="s">
         <v>890</v>
       </c>
-      <c r="G14" s="203"/>
-      <c r="H14" s="203"/>
+      <c r="G14" s="202"/>
+      <c r="H14" s="202"/>
       <c r="I14" s="79" t="s">
         <v>1131</v>
       </c>
@@ -9410,8 +9419,8 @@
       <c r="E25" s="199" t="s">
         <v>341</v>
       </c>
-      <c r="F25" s="202"/>
-      <c r="G25" s="200"/>
+      <c r="F25" s="200"/>
+      <c r="G25" s="201"/>
       <c r="H25" s="75" t="s">
         <v>1133</v>
       </c>
@@ -9471,12 +9480,12 @@
       <c r="D29" s="199" t="s">
         <v>345</v>
       </c>
-      <c r="E29" s="200"/>
+      <c r="E29" s="201"/>
       <c r="F29" s="199" t="s">
         <v>347</v>
       </c>
-      <c r="G29" s="202"/>
-      <c r="H29" s="200"/>
+      <c r="G29" s="200"/>
+      <c r="H29" s="201"/>
       <c r="I29" s="81"/>
       <c r="J29" s="75"/>
     </row>
@@ -9484,15 +9493,15 @@
       <c r="C30" s="76">
         <v>13473</v>
       </c>
-      <c r="D30" s="203" t="s">
+      <c r="D30" s="202" t="s">
         <v>909</v>
       </c>
-      <c r="E30" s="203"/>
-      <c r="F30" s="203" t="s">
+      <c r="E30" s="202"/>
+      <c r="F30" s="202" t="s">
         <v>888</v>
       </c>
-      <c r="G30" s="203"/>
-      <c r="H30" s="203"/>
+      <c r="G30" s="202"/>
+      <c r="H30" s="202"/>
       <c r="I30" s="79" t="s">
         <v>1131</v>
       </c>
@@ -9504,15 +9513,15 @@
       <c r="C31" s="76">
         <v>13474</v>
       </c>
-      <c r="D31" s="203" t="s">
+      <c r="D31" s="202" t="s">
         <v>931</v>
       </c>
-      <c r="E31" s="203"/>
-      <c r="F31" s="203" t="s">
+      <c r="E31" s="202"/>
+      <c r="F31" s="202" t="s">
         <v>890</v>
       </c>
-      <c r="G31" s="203"/>
-      <c r="H31" s="203"/>
+      <c r="G31" s="202"/>
+      <c r="H31" s="202"/>
       <c r="I31" s="79" t="s">
         <v>1131</v>
       </c>
@@ -9531,11 +9540,11 @@
       <c r="D33" s="199" t="s">
         <v>365</v>
       </c>
-      <c r="E33" s="200"/>
+      <c r="E33" s="201"/>
       <c r="F33" s="199" t="s">
         <v>175</v>
       </c>
-      <c r="G33" s="200"/>
+      <c r="G33" s="201"/>
       <c r="H33" s="82" t="s">
         <v>176</v>
       </c>
@@ -9546,14 +9555,14 @@
       <c r="C34" s="76">
         <v>1454</v>
       </c>
-      <c r="D34" s="203" t="s">
+      <c r="D34" s="202" t="s">
         <v>1150</v>
       </c>
-      <c r="E34" s="203"/>
-      <c r="F34" s="204">
+      <c r="E34" s="202"/>
+      <c r="F34" s="203">
         <v>43133</v>
       </c>
-      <c r="G34" s="204"/>
+      <c r="G34" s="203"/>
       <c r="H34" s="85">
         <v>43134</v>
       </c>
@@ -9568,14 +9577,14 @@
       <c r="C35" s="76">
         <v>1455</v>
       </c>
-      <c r="D35" s="203" t="s">
+      <c r="D35" s="202" t="s">
         <v>1150</v>
       </c>
-      <c r="E35" s="203"/>
-      <c r="F35" s="204">
+      <c r="E35" s="202"/>
+      <c r="F35" s="203">
         <v>43132</v>
       </c>
-      <c r="G35" s="204"/>
+      <c r="G35" s="203"/>
       <c r="H35" s="85">
         <v>43159</v>
       </c>
@@ -9591,6 +9600,24 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="D33:E33"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F30:H30"/>
@@ -9598,24 +9625,6 @@
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15181,11 +15190,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AA209"/>
+  <dimension ref="A1:AA210"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <pane ySplit="8" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15419,7 +15428,7 @@
         <v>153</v>
       </c>
       <c r="C11" s="23" t="str">
-        <f t="shared" ref="C11:C22" si="0">"Submission." &amp; B11</f>
+        <f t="shared" ref="C11:C24" si="0">"Submission." &amp; B11</f>
         <v>Submission.LPR003</v>
       </c>
       <c r="D11" s="109" t="s">
@@ -15927,17 +15936,17 @@
     <row r="22" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
       <c r="B22" s="179" t="s">
-        <v>1572</v>
+        <v>1589</v>
       </c>
       <c r="C22" s="179" t="str">
-        <f t="shared" si="0"/>
-        <v>Submission.LPR100</v>
+        <f>"Submission." &amp; B22</f>
+        <v>Submission.LPR103</v>
       </c>
       <c r="D22" s="180" t="s">
-        <v>1582</v>
-      </c>
-      <c r="E22" s="182" t="s">
-        <v>1573</v>
+        <v>1018</v>
+      </c>
+      <c r="E22" s="181" t="s">
+        <v>1590</v>
       </c>
       <c r="F22" s="183"/>
       <c r="G22" s="183"/>
@@ -15964,17 +15973,17 @@
     <row r="23" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
       <c r="B23" s="179" t="s">
-        <v>1578</v>
+        <v>1580</v>
       </c>
       <c r="C23" s="179" t="str">
         <f t="shared" ref="C23" si="1">"Submission." &amp; B23</f>
-        <v>Submission.LPR101</v>
+        <v>Submission.LPR102</v>
       </c>
       <c r="D23" s="180" t="s">
-        <v>1581</v>
+        <v>902</v>
       </c>
       <c r="E23" s="181" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="F23" s="183"/>
       <c r="G23" s="183"/>
@@ -16001,17 +16010,17 @@
     <row r="24" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
       <c r="B24" s="179" t="s">
-        <v>1580</v>
+        <v>1572</v>
       </c>
       <c r="C24" s="179" t="str">
-        <f t="shared" ref="C24" si="2">"Submission." &amp; B24</f>
-        <v>Submission.LPR102</v>
+        <f t="shared" si="0"/>
+        <v>Submission.LPR100</v>
       </c>
       <c r="D24" s="180" t="s">
-        <v>902</v>
-      </c>
-      <c r="E24" s="181" t="s">
-        <v>1584</v>
+        <v>1582</v>
+      </c>
+      <c r="E24" s="182" t="s">
+        <v>1573</v>
       </c>
       <c r="F24" s="183"/>
       <c r="G24" s="183"/>
@@ -16038,17 +16047,17 @@
     <row r="25" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
       <c r="B25" s="179" t="s">
-        <v>1589</v>
+        <v>1578</v>
       </c>
       <c r="C25" s="179" t="str">
-        <f>"Submission." &amp; B25</f>
-        <v>Submission.LPR103</v>
+        <f t="shared" ref="C25" si="2">"Submission." &amp; B25</f>
+        <v>Submission.LPR101</v>
       </c>
       <c r="D25" s="180" t="s">
-        <v>1018</v>
+        <v>1581</v>
       </c>
       <c r="E25" s="181" t="s">
-        <v>1590</v>
+        <v>1583</v>
       </c>
       <c r="F25" s="183"/>
       <c r="G25" s="183"/>
@@ -20393,7 +20402,7 @@
         <v>1271</v>
       </c>
       <c r="M120" s="123" t="b">
-        <f>AND(ABS(H120-H14)&lt;=H204,ABS(H14-H120)&lt;=H204)</f>
+        <f>AND(ABS(H120-H14)&lt;=H205,ABS(H14-H120)&lt;=H205)</f>
         <v>1</v>
       </c>
       <c r="N120" s="10" t="s">
@@ -20451,7 +20460,7 @@
         <v>1381</v>
       </c>
       <c r="O121" s="123" t="b">
-        <f>AND(ABS(H121-H14)&lt;=H204,ABS(H14-H121)&lt;=H204)</f>
+        <f>AND(ABS(H121-H14)&lt;=H205,ABS(H14-H121)&lt;=H205)</f>
         <v>1</v>
       </c>
       <c r="P121" s="10" t="s">
@@ -21182,7 +21191,7 @@
         <v>370</v>
       </c>
       <c r="C138" s="119" t="str">
-        <f t="shared" ref="C138:C167" si="8">"Loan." &amp; B138</f>
+        <f t="shared" ref="C138:C168" si="8">"Loan." &amp; B138</f>
         <v>Loan.LPL001a</v>
       </c>
       <c r="D138" s="109" t="s">
@@ -21860,7 +21869,7 @@
         <v>1484</v>
       </c>
       <c r="O151" s="123" t="b">
-        <f>AND(ABS(H151-I13)&lt;=H204,ABS(I13-H151)&lt;=H204)</f>
+        <f>AND(ABS(H151-I13)&lt;=H205,ABS(I13-H151)&lt;=H205)</f>
         <v>0</v>
       </c>
       <c r="P151" s="10" t="s">
@@ -21916,7 +21925,7 @@
         <v>1486</v>
       </c>
       <c r="O152" s="123" t="b">
-        <f>AND(ABS(JH152-I13)&lt;=H205,ABS(I13-H152)&lt;=H204)</f>
+        <f>AND(ABS(JH152-I13)&lt;=H206,ABS(I13-H152)&lt;=H205)</f>
         <v>0</v>
       </c>
       <c r="P152" s="10" t="s">
@@ -22549,7 +22558,7 @@
         <v>1503</v>
       </c>
       <c r="O165" s="123" t="b">
-        <f>AND(ABS(JH165-I27)&lt;=H204,ABS(I13-H165)&lt;=H204)</f>
+        <f>AND(ABS(JH165-I27)&lt;=H205,ABS(I13-H165)&lt;=H205)</f>
         <v>0</v>
       </c>
       <c r="P165" s="10" t="s">
@@ -22653,64 +22662,54 @@
       <c r="Y167" s="29"/>
       <c r="Z167" s="10"/>
     </row>
-    <row r="168" spans="1:27" ht="45.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="15"/>
-      <c r="B168" s="108" t="s">
-        <v>62</v>
+      <c r="B168" s="179" t="s">
+        <v>1616</v>
       </c>
       <c r="C168" s="119" t="str">
-        <f>"LoanCovenant." &amp; B168</f>
-        <v>LoanCovenant.LPC001</v>
-      </c>
-      <c r="D168" s="109" t="s">
-        <v>1508</v>
-      </c>
-      <c r="E168" s="108" t="s">
-        <v>139</v>
-      </c>
-      <c r="F168" s="108" t="s">
-        <v>1268</v>
-      </c>
-      <c r="G168" s="109" t="s">
-        <v>1519</v>
-      </c>
-      <c r="H168" s="103"/>
-      <c r="I168" s="120">
-        <f>I138</f>
-        <v>1</v>
-      </c>
-      <c r="J168" s="120"/>
-      <c r="K168" s="108"/>
-      <c r="L168" s="109"/>
+        <f t="shared" si="8"/>
+        <v>Loan.LPL101</v>
+      </c>
+      <c r="D168" s="180" t="s">
+        <v>1617</v>
+      </c>
+      <c r="E168" s="182" t="s">
+        <v>1618</v>
+      </c>
+      <c r="F168" s="183"/>
+      <c r="G168" s="183"/>
+      <c r="H168" s="184"/>
+      <c r="I168" s="185"/>
+      <c r="J168" s="180"/>
+      <c r="K168" s="9"/>
+      <c r="L168" s="10"/>
       <c r="M168" s="102"/>
-      <c r="N168" s="109"/>
+      <c r="N168" s="10"/>
       <c r="O168" s="102"/>
-      <c r="P168" s="109"/>
+      <c r="P168" s="10"/>
       <c r="Q168" s="102"/>
-      <c r="R168" s="109"/>
+      <c r="R168" s="10"/>
       <c r="S168" s="102"/>
-      <c r="T168" s="109"/>
+      <c r="T168" s="10"/>
       <c r="U168" s="102"/>
-      <c r="V168" s="109"/>
-      <c r="W168" s="109"/>
-      <c r="X168" s="109"/>
-      <c r="Y168" s="109" t="s">
-        <v>308</v>
-      </c>
-      <c r="Z168" s="17"/>
-      <c r="AA168" s="86"/>
+      <c r="V168" s="10"/>
+      <c r="W168" s="162"/>
+      <c r="X168" s="162"/>
+      <c r="Y168" s="29"/>
+      <c r="Z168" s="10"/>
     </row>
     <row r="169" spans="1:27" ht="45.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="15"/>
       <c r="B169" s="108" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C169" s="119" t="str">
-        <f t="shared" ref="C169:C176" si="9">"LoanCovenant." &amp; B169</f>
-        <v>LoanCovenant.LPC002</v>
+        <f>"LoanCovenant." &amp; B169</f>
+        <v>LoanCovenant.LPC001</v>
       </c>
       <c r="D169" s="109" t="s">
-        <v>1520</v>
+        <v>1508</v>
       </c>
       <c r="E169" s="108" t="s">
         <v>139</v>
@@ -22719,12 +22718,12 @@
         <v>1268</v>
       </c>
       <c r="G169" s="109" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="H169" s="103"/>
-      <c r="I169" s="120" t="str">
-        <f>I140</f>
-        <v>BOSFIXED0001</v>
+      <c r="I169" s="120">
+        <f>I138</f>
+        <v>1</v>
       </c>
       <c r="J169" s="120"/>
       <c r="K169" s="108"/>
@@ -22742,7 +22741,7 @@
       <c r="W169" s="109"/>
       <c r="X169" s="109"/>
       <c r="Y169" s="109" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Z169" s="17"/>
       <c r="AA169" s="86"/>
@@ -22750,28 +22749,28 @@
     <row r="170" spans="1:27" ht="45.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="15"/>
       <c r="B170" s="108" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C170" s="119" t="str">
-        <f t="shared" si="9"/>
-        <v>LoanCovenant.LPC003</v>
+        <f t="shared" ref="C170:C177" si="9">"LoanCovenant." &amp; B170</f>
+        <v>LoanCovenant.LPC002</v>
       </c>
       <c r="D170" s="109" t="s">
-        <v>1342</v>
+        <v>1520</v>
       </c>
       <c r="E170" s="108" t="s">
-        <v>1277</v>
+        <v>139</v>
       </c>
       <c r="F170" s="108" t="s">
         <v>1268</v>
       </c>
       <c r="G170" s="109" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="H170" s="103"/>
-      <c r="I170" s="107">
-        <f>Pfo_Page_Serial</f>
-        <v>1</v>
+      <c r="I170" s="120" t="str">
+        <f>I140</f>
+        <v>BOSFIXED0001</v>
       </c>
       <c r="J170" s="120"/>
       <c r="K170" s="108"/>
@@ -22789,75 +22788,78 @@
       <c r="W170" s="109"/>
       <c r="X170" s="109"/>
       <c r="Y170" s="109" t="s">
-        <v>310</v>
-      </c>
-      <c r="Z170" s="17" t="s">
-        <v>907</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="Z170" s="17"/>
       <c r="AA170" s="86"/>
     </row>
-    <row r="171" spans="1:27" ht="92.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B171" s="23" t="s">
-        <v>65</v>
+    <row r="171" spans="1:27" ht="45.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="15"/>
+      <c r="B171" s="108" t="s">
+        <v>64</v>
       </c>
       <c r="C171" s="119" t="str">
         <f t="shared" si="9"/>
-        <v>LoanCovenant.LPC004</v>
-      </c>
-      <c r="D171" s="16" t="s">
-        <v>345</v>
-      </c>
-      <c r="E171" s="23" t="s">
-        <v>1585</v>
-      </c>
-      <c r="F171" s="17"/>
-      <c r="G171" s="17"/>
-      <c r="H171" s="104" t="s">
-        <v>921</v>
-      </c>
-      <c r="I171" s="105"/>
+        <v>LoanCovenant.LPC003</v>
+      </c>
+      <c r="D171" s="109" t="s">
+        <v>1342</v>
+      </c>
+      <c r="E171" s="108" t="s">
+        <v>1277</v>
+      </c>
+      <c r="F171" s="108" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G171" s="109" t="s">
+        <v>1523</v>
+      </c>
+      <c r="H171" s="103"/>
+      <c r="I171" s="107">
+        <f>Pfo_Page_Serial</f>
+        <v>1</v>
+      </c>
       <c r="J171" s="120"/>
-      <c r="K171" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="L171" s="10"/>
+      <c r="K171" s="108"/>
+      <c r="L171" s="109"/>
       <c r="M171" s="102"/>
-      <c r="N171" s="10"/>
+      <c r="N171" s="109"/>
       <c r="O171" s="102"/>
-      <c r="P171" s="10"/>
+      <c r="P171" s="109"/>
       <c r="Q171" s="102"/>
-      <c r="R171" s="10"/>
+      <c r="R171" s="109"/>
       <c r="S171" s="102"/>
-      <c r="T171" s="10"/>
+      <c r="T171" s="109"/>
       <c r="U171" s="102"/>
-      <c r="V171" s="10"/>
-      <c r="W171" s="10"/>
-      <c r="X171" s="10"/>
-      <c r="Y171" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="Z171" s="10" t="s">
-        <v>415</v>
-      </c>
+      <c r="V171" s="109"/>
+      <c r="W171" s="109"/>
+      <c r="X171" s="109"/>
+      <c r="Y171" s="109" t="s">
+        <v>310</v>
+      </c>
+      <c r="Z171" s="17" t="s">
+        <v>907</v>
+      </c>
+      <c r="AA171" s="86"/>
     </row>
     <row r="172" spans="1:27" ht="92.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B172" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C172" s="119" t="str">
         <f t="shared" si="9"/>
-        <v>LoanCovenant.LPC005</v>
+        <v>LoanCovenant.LPC004</v>
       </c>
       <c r="D172" s="16" t="s">
-        <v>174</v>
+        <v>345</v>
       </c>
       <c r="E172" s="23" t="s">
-        <v>138</v>
+        <v>1585</v>
       </c>
       <c r="F172" s="17"/>
       <c r="G172" s="17"/>
       <c r="H172" s="104" t="s">
-        <v>1525</v>
+        <v>921</v>
       </c>
       <c r="I172" s="105"/>
       <c r="J172" s="120"/>
@@ -22866,9 +22868,7 @@
       </c>
       <c r="L172" s="10"/>
       <c r="M172" s="102"/>
-      <c r="N172" s="10" t="s">
-        <v>1524</v>
-      </c>
+      <c r="N172" s="10"/>
       <c r="O172" s="102"/>
       <c r="P172" s="10"/>
       <c r="Q172" s="102"/>
@@ -22880,28 +22880,30 @@
       <c r="W172" s="10"/>
       <c r="X172" s="10"/>
       <c r="Y172" s="16" t="s">
-        <v>312</v>
-      </c>
-      <c r="Z172" s="10"/>
+        <v>311</v>
+      </c>
+      <c r="Z172" s="10" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="173" spans="1:27" ht="92.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B173" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C173" s="119" t="str">
         <f t="shared" si="9"/>
-        <v>LoanCovenant.LPC006</v>
+        <v>LoanCovenant.LPC005</v>
       </c>
       <c r="D173" s="16" t="s">
-        <v>346</v>
+        <v>174</v>
       </c>
       <c r="E173" s="23" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F173" s="17"/>
       <c r="G173" s="17"/>
-      <c r="H173" s="149" t="s">
-        <v>1526</v>
+      <c r="H173" s="104" t="s">
+        <v>1525</v>
       </c>
       <c r="I173" s="105"/>
       <c r="J173" s="120"/>
@@ -22910,7 +22912,9 @@
       </c>
       <c r="L173" s="10"/>
       <c r="M173" s="102"/>
-      <c r="N173" s="10"/>
+      <c r="N173" s="10" t="s">
+        <v>1524</v>
+      </c>
       <c r="O173" s="102"/>
       <c r="P173" s="10"/>
       <c r="Q173" s="102"/>
@@ -22922,30 +22926,28 @@
       <c r="W173" s="10"/>
       <c r="X173" s="10"/>
       <c r="Y173" s="16" t="s">
-        <v>313</v>
-      </c>
-      <c r="Z173" s="10" t="s">
-        <v>973</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="Z173" s="10"/>
     </row>
     <row r="174" spans="1:27" ht="92.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B174" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C174" s="119" t="str">
         <f t="shared" si="9"/>
-        <v>LoanCovenant.LPC007</v>
+        <v>LoanCovenant.LPC006</v>
       </c>
       <c r="D174" s="16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E174" s="23" t="s">
-        <v>1512</v>
+        <v>136</v>
       </c>
       <c r="F174" s="17"/>
       <c r="G174" s="17"/>
-      <c r="H174" s="104" t="s">
-        <v>888</v>
+      <c r="H174" s="149" t="s">
+        <v>1526</v>
       </c>
       <c r="I174" s="105"/>
       <c r="J174" s="120"/>
@@ -22966,30 +22968,30 @@
       <c r="W174" s="10"/>
       <c r="X174" s="10"/>
       <c r="Y174" s="16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Z174" s="10" t="s">
-        <v>415</v>
+        <v>973</v>
       </c>
     </row>
     <row r="175" spans="1:27" ht="92.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B175" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C175" s="119" t="str">
         <f t="shared" si="9"/>
-        <v>LoanCovenant.LPC008</v>
+        <v>LoanCovenant.LPC007</v>
       </c>
       <c r="D175" s="16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E175" s="23" t="s">
-        <v>132</v>
+        <v>1512</v>
       </c>
       <c r="F175" s="17"/>
       <c r="G175" s="17"/>
-      <c r="H175" s="104">
-        <v>40269</v>
+      <c r="H175" s="104" t="s">
+        <v>888</v>
       </c>
       <c r="I175" s="105"/>
       <c r="J175" s="120"/>
@@ -23010,30 +23012,30 @@
       <c r="W175" s="10"/>
       <c r="X175" s="10"/>
       <c r="Y175" s="16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Z175" s="10" t="s">
-        <v>1231</v>
+        <v>415</v>
       </c>
     </row>
     <row r="176" spans="1:27" ht="92.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B176" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C176" s="119" t="str">
         <f t="shared" si="9"/>
-        <v>LoanCovenant.LPC009</v>
+        <v>LoanCovenant.LPC008</v>
       </c>
       <c r="D176" s="16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E176" s="23" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F176" s="17"/>
       <c r="G176" s="17"/>
-      <c r="H176" s="149" t="s">
-        <v>1527</v>
+      <c r="H176" s="104">
+        <v>40269</v>
       </c>
       <c r="I176" s="105"/>
       <c r="J176" s="120"/>
@@ -23054,100 +23056,97 @@
       <c r="W176" s="10"/>
       <c r="X176" s="10"/>
       <c r="Y176" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="Z176" s="10" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="177" spans="1:27" ht="92.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B177" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C177" s="119" t="str">
+        <f t="shared" si="9"/>
+        <v>LoanCovenant.LPC009</v>
+      </c>
+      <c r="D177" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="E177" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="F177" s="17"/>
+      <c r="G177" s="17"/>
+      <c r="H177" s="149" t="s">
+        <v>1527</v>
+      </c>
+      <c r="I177" s="105"/>
+      <c r="J177" s="120"/>
+      <c r="K177" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="L177" s="10"/>
+      <c r="M177" s="102"/>
+      <c r="N177" s="10"/>
+      <c r="O177" s="102"/>
+      <c r="P177" s="10"/>
+      <c r="Q177" s="102"/>
+      <c r="R177" s="10"/>
+      <c r="S177" s="102"/>
+      <c r="T177" s="10"/>
+      <c r="U177" s="102"/>
+      <c r="V177" s="10"/>
+      <c r="W177" s="10"/>
+      <c r="X177" s="10"/>
+      <c r="Y177" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="Z176" s="10" t="s">
+      <c r="Z177" s="10" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="177" spans="1:27" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A177" s="15"/>
-      <c r="B177" s="24"/>
-      <c r="C177" s="36" t="s">
+    <row r="178" spans="1:27" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A178" s="15"/>
+      <c r="B178" s="24"/>
+      <c r="C178" s="36" t="s">
         <v>1021</v>
       </c>
-      <c r="D177" s="12"/>
-      <c r="E177" s="12"/>
-      <c r="F177" s="12"/>
-      <c r="G177" s="12"/>
-      <c r="H177" s="12"/>
-      <c r="I177" s="12"/>
-      <c r="J177" s="12"/>
-      <c r="K177" s="12"/>
-      <c r="L177" s="12"/>
-      <c r="M177" s="12"/>
-      <c r="N177" s="12"/>
-      <c r="O177" s="12"/>
-      <c r="P177" s="12"/>
-      <c r="Q177" s="12"/>
-      <c r="R177" s="12"/>
-      <c r="S177" s="12"/>
-      <c r="T177" s="12"/>
-      <c r="U177" s="12"/>
-      <c r="V177" s="12"/>
-      <c r="W177" s="163"/>
-      <c r="X177" s="163"/>
-      <c r="Y177" s="35"/>
-      <c r="Z177" s="14"/>
-    </row>
-    <row r="178" spans="1:27" ht="45.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="15"/>
-      <c r="B178" s="108" t="s">
-        <v>71</v>
-      </c>
-      <c r="C178" s="119" t="str">
-        <f>"EIRD." &amp; B178</f>
-        <v>EIRD.LPC010</v>
-      </c>
-      <c r="D178" s="109" t="s">
-        <v>1508</v>
-      </c>
-      <c r="E178" s="108" t="s">
-        <v>139</v>
-      </c>
-      <c r="F178" s="108" t="s">
-        <v>1268</v>
-      </c>
-      <c r="G178" s="109" t="s">
-        <v>1519</v>
-      </c>
-      <c r="H178" s="103"/>
-      <c r="I178" s="120">
-        <f>I138</f>
-        <v>1</v>
-      </c>
-      <c r="J178" s="120"/>
-      <c r="K178" s="108"/>
-      <c r="L178" s="109"/>
-      <c r="M178" s="102"/>
-      <c r="N178" s="109"/>
-      <c r="O178" s="102"/>
-      <c r="P178" s="109"/>
-      <c r="Q178" s="102"/>
-      <c r="R178" s="109"/>
-      <c r="S178" s="102"/>
-      <c r="T178" s="109"/>
-      <c r="U178" s="102"/>
-      <c r="V178" s="109"/>
-      <c r="W178" s="109"/>
-      <c r="X178" s="109"/>
-      <c r="Y178" s="109" t="s">
-        <v>317</v>
-      </c>
-      <c r="Z178" s="17"/>
-      <c r="AA178" s="86"/>
+      <c r="D178" s="12"/>
+      <c r="E178" s="12"/>
+      <c r="F178" s="12"/>
+      <c r="G178" s="12"/>
+      <c r="H178" s="12"/>
+      <c r="I178" s="12"/>
+      <c r="J178" s="12"/>
+      <c r="K178" s="12"/>
+      <c r="L178" s="12"/>
+      <c r="M178" s="12"/>
+      <c r="N178" s="12"/>
+      <c r="O178" s="12"/>
+      <c r="P178" s="12"/>
+      <c r="Q178" s="12"/>
+      <c r="R178" s="12"/>
+      <c r="S178" s="12"/>
+      <c r="T178" s="12"/>
+      <c r="U178" s="12"/>
+      <c r="V178" s="12"/>
+      <c r="W178" s="163"/>
+      <c r="X178" s="163"/>
+      <c r="Y178" s="35"/>
+      <c r="Z178" s="14"/>
     </row>
     <row r="179" spans="1:27" ht="45.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="15"/>
       <c r="B179" s="108" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C179" s="119" t="str">
-        <f t="shared" ref="C179:C187" si="10">"EIRD." &amp; B179</f>
-        <v>EIRD.LPC012</v>
+        <f>"EIRD." &amp; B179</f>
+        <v>EIRD.LPC010</v>
       </c>
       <c r="D179" s="109" t="s">
-        <v>1528</v>
+        <v>1508</v>
       </c>
       <c r="E179" s="108" t="s">
         <v>139</v>
@@ -23156,12 +23155,12 @@
         <v>1268</v>
       </c>
       <c r="G179" s="109" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="H179" s="103"/>
-      <c r="I179" s="120" t="str">
-        <f>I140</f>
-        <v>BOSFIXED0001</v>
+      <c r="I179" s="120">
+        <f>I138</f>
+        <v>1</v>
       </c>
       <c r="J179" s="120"/>
       <c r="K179" s="108"/>
@@ -23179,7 +23178,7 @@
       <c r="W179" s="109"/>
       <c r="X179" s="109"/>
       <c r="Y179" s="109" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Z179" s="17"/>
       <c r="AA179" s="86"/>
@@ -23187,28 +23186,28 @@
     <row r="180" spans="1:27" ht="45.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="15"/>
       <c r="B180" s="108" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C180" s="119" t="str">
-        <f t="shared" si="10"/>
-        <v>EIRD.LPC013</v>
+        <f t="shared" ref="C180:C188" si="10">"EIRD." &amp; B180</f>
+        <v>EIRD.LPC012</v>
       </c>
       <c r="D180" s="109" t="s">
-        <v>1342</v>
+        <v>1528</v>
       </c>
       <c r="E180" s="108" t="s">
-        <v>1277</v>
+        <v>139</v>
       </c>
       <c r="F180" s="108" t="s">
         <v>1268</v>
       </c>
       <c r="G180" s="109" t="s">
-        <v>1532</v>
+        <v>1521</v>
       </c>
       <c r="H180" s="103"/>
-      <c r="I180" s="107">
-        <f>Pfo_Page_Serial</f>
-        <v>1</v>
+      <c r="I180" s="120" t="str">
+        <f>I140</f>
+        <v>BOSFIXED0001</v>
       </c>
       <c r="J180" s="120"/>
       <c r="K180" s="108"/>
@@ -23226,77 +23225,79 @@
       <c r="W180" s="109"/>
       <c r="X180" s="109"/>
       <c r="Y180" s="109" t="s">
-        <v>319</v>
-      </c>
-      <c r="Z180" s="17" t="s">
-        <v>907</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="Z180" s="17"/>
       <c r="AA180" s="86"/>
     </row>
-    <row r="181" spans="1:27" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:27" ht="45.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="15"/>
-      <c r="B181" s="23" t="s">
-        <v>74</v>
+      <c r="B181" s="108" t="s">
+        <v>73</v>
       </c>
       <c r="C181" s="119" t="str">
         <f t="shared" si="10"/>
-        <v>EIRD.LPC014</v>
-      </c>
-      <c r="D181" s="16" t="s">
-        <v>1534</v>
-      </c>
-      <c r="E181" s="23" t="s">
-        <v>1610</v>
-      </c>
-      <c r="F181" s="17"/>
-      <c r="G181" s="17"/>
-      <c r="H181" s="149" t="s">
-        <v>1014</v>
-      </c>
-      <c r="I181" s="105"/>
+        <v>EIRD.LPC013</v>
+      </c>
+      <c r="D181" s="109" t="s">
+        <v>1342</v>
+      </c>
+      <c r="E181" s="108" t="s">
+        <v>1277</v>
+      </c>
+      <c r="F181" s="108" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G181" s="109" t="s">
+        <v>1532</v>
+      </c>
+      <c r="H181" s="103"/>
+      <c r="I181" s="107">
+        <f>Pfo_Page_Serial</f>
+        <v>1</v>
+      </c>
       <c r="J181" s="120"/>
-      <c r="K181" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="L181" s="10"/>
+      <c r="K181" s="108"/>
+      <c r="L181" s="109"/>
       <c r="M181" s="102"/>
-      <c r="N181" s="10"/>
+      <c r="N181" s="109"/>
       <c r="O181" s="102"/>
-      <c r="P181" s="10"/>
+      <c r="P181" s="109"/>
       <c r="Q181" s="102"/>
-      <c r="R181" s="10"/>
+      <c r="R181" s="109"/>
       <c r="S181" s="102"/>
-      <c r="T181" s="10"/>
+      <c r="T181" s="109"/>
       <c r="U181" s="102"/>
-      <c r="V181" s="10"/>
-      <c r="W181" s="10"/>
-      <c r="X181" s="10"/>
-      <c r="Y181" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="Z181" s="10" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="182" spans="1:27" s="18" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V181" s="109"/>
+      <c r="W181" s="109"/>
+      <c r="X181" s="109"/>
+      <c r="Y181" s="109" t="s">
+        <v>319</v>
+      </c>
+      <c r="Z181" s="17" t="s">
+        <v>907</v>
+      </c>
+      <c r="AA181" s="86"/>
+    </row>
+    <row r="182" spans="1:27" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A182" s="15"/>
       <c r="B182" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C182" s="119" t="str">
         <f t="shared" si="10"/>
-        <v>EIRD.LPC015</v>
+        <v>EIRD.LPC014</v>
       </c>
       <c r="D182" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="E182" s="9" t="s">
-        <v>1305</v>
+        <v>1534</v>
+      </c>
+      <c r="E182" s="23" t="s">
+        <v>1610</v>
       </c>
       <c r="F182" s="17"/>
       <c r="G182" s="17"/>
-      <c r="H182" s="103">
-        <v>5000</v>
+      <c r="H182" s="149" t="s">
+        <v>1014</v>
       </c>
       <c r="I182" s="105"/>
       <c r="J182" s="120"/>
@@ -23317,29 +23318,31 @@
       <c r="W182" s="10"/>
       <c r="X182" s="10"/>
       <c r="Y182" s="16" t="s">
-        <v>321</v>
-      </c>
-      <c r="Z182" s="10"/>
-    </row>
-    <row r="183" spans="1:27" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>320</v>
+      </c>
+      <c r="Z182" s="10" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="183" spans="1:27" s="18" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="15"/>
       <c r="B183" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C183" s="119" t="str">
         <f t="shared" si="10"/>
-        <v>EIRD.LPC016</v>
+        <v>EIRD.LPC015</v>
       </c>
       <c r="D183" s="16" t="s">
-        <v>1535</v>
-      </c>
-      <c r="E183" s="23" t="s">
-        <v>132</v>
+        <v>178</v>
+      </c>
+      <c r="E183" s="9" t="s">
+        <v>1305</v>
       </c>
       <c r="F183" s="17"/>
       <c r="G183" s="17"/>
-      <c r="H183" s="106">
-        <v>38443</v>
+      <c r="H183" s="103">
+        <v>5000</v>
       </c>
       <c r="I183" s="105"/>
       <c r="J183" s="120"/>
@@ -23360,23 +23363,21 @@
       <c r="W183" s="10"/>
       <c r="X183" s="10"/>
       <c r="Y183" s="16" t="s">
-        <v>322</v>
-      </c>
-      <c r="Z183" s="10" t="s">
-        <v>1231</v>
-      </c>
-    </row>
-    <row r="184" spans="1:27" s="18" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+      <c r="Z183" s="10"/>
+    </row>
+    <row r="184" spans="1:27" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A184" s="15"/>
       <c r="B184" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C184" s="119" t="str">
         <f t="shared" si="10"/>
-        <v>EIRD.LPC017</v>
+        <v>EIRD.LPC016</v>
       </c>
       <c r="D184" s="16" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="E184" s="23" t="s">
         <v>132</v>
@@ -23384,7 +23385,7 @@
       <c r="F184" s="17"/>
       <c r="G184" s="17"/>
       <c r="H184" s="106">
-        <v>42094</v>
+        <v>38443</v>
       </c>
       <c r="I184" s="105"/>
       <c r="J184" s="120"/>
@@ -23392,13 +23393,8 @@
         <v>133</v>
       </c>
       <c r="L184" s="10"/>
-      <c r="M184" s="102" t="b">
-        <f>H184&gt;=H183</f>
-        <v>1</v>
-      </c>
-      <c r="N184" s="10" t="s">
-        <v>1531</v>
-      </c>
+      <c r="M184" s="102"/>
+      <c r="N184" s="10"/>
       <c r="O184" s="102"/>
       <c r="P184" s="10"/>
       <c r="Q184" s="102"/>
@@ -23410,39 +23406,45 @@
       <c r="W184" s="10"/>
       <c r="X184" s="10"/>
       <c r="Y184" s="16" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Z184" s="10" t="s">
         <v>1231</v>
       </c>
     </row>
-    <row r="185" spans="1:27" s="18" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:27" s="18" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="15"/>
       <c r="B185" s="23" t="s">
-        <v>1530</v>
+        <v>77</v>
       </c>
       <c r="C185" s="119" t="str">
         <f t="shared" si="10"/>
-        <v>EIRD.LPC018a</v>
+        <v>EIRD.LPC017</v>
       </c>
       <c r="D185" s="16" t="s">
-        <v>1537</v>
-      </c>
-      <c r="E185" s="9" t="s">
-        <v>1310</v>
+        <v>1536</v>
+      </c>
+      <c r="E185" s="23" t="s">
+        <v>132</v>
       </c>
       <c r="F185" s="17"/>
       <c r="G185" s="17"/>
-      <c r="H185" s="151">
-        <v>20.0001</v>
+      <c r="H185" s="106">
+        <v>42094</v>
       </c>
       <c r="I185" s="105"/>
-      <c r="J185" s="101"/>
+      <c r="J185" s="120"/>
       <c r="K185" s="9" t="s">
         <v>133</v>
       </c>
       <c r="L185" s="10"/>
-      <c r="M185" s="102"/>
-      <c r="N185" s="10"/>
+      <c r="M185" s="102" t="b">
+        <f>H185&gt;=H184</f>
+        <v>1</v>
+      </c>
+      <c r="N185" s="10" t="s">
+        <v>1531</v>
+      </c>
       <c r="O185" s="102"/>
       <c r="P185" s="10"/>
       <c r="Q185" s="102"/>
@@ -23454,20 +23456,22 @@
       <c r="W185" s="10"/>
       <c r="X185" s="10"/>
       <c r="Y185" s="16" t="s">
-        <v>324</v>
-      </c>
-      <c r="Z185" s="10"/>
-    </row>
-    <row r="186" spans="1:27" s="18" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+      <c r="Z185" s="10" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="186" spans="1:27" s="18" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B186" s="23" t="s">
-        <v>392</v>
+        <v>1530</v>
       </c>
       <c r="C186" s="119" t="str">
         <f t="shared" si="10"/>
-        <v>EIRD.LPC018b</v>
+        <v>EIRD.LPC018a</v>
       </c>
       <c r="D186" s="16" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="E186" s="9" t="s">
         <v>1310</v>
@@ -23475,7 +23479,7 @@
       <c r="F186" s="17"/>
       <c r="G186" s="17"/>
       <c r="H186" s="151">
-        <v>3.875</v>
+        <v>20.0001</v>
       </c>
       <c r="I186" s="105"/>
       <c r="J186" s="101"/>
@@ -23500,24 +23504,24 @@
       </c>
       <c r="Z186" s="10"/>
     </row>
-    <row r="187" spans="1:27" s="18" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:27" s="18" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B187" s="23" t="s">
-        <v>1614</v>
+        <v>392</v>
       </c>
       <c r="C187" s="119" t="str">
         <f t="shared" si="10"/>
-        <v>EIRD.LPC018c</v>
+        <v>EIRD.LPC018b</v>
       </c>
       <c r="D187" s="16" t="s">
-        <v>1539</v>
-      </c>
-      <c r="E187" s="23" t="s">
-        <v>398</v>
+        <v>1538</v>
+      </c>
+      <c r="E187" s="9" t="s">
+        <v>1310</v>
       </c>
       <c r="F187" s="17"/>
       <c r="G187" s="17"/>
-      <c r="H187" s="116" t="b">
-        <v>1</v>
+      <c r="H187" s="151">
+        <v>3.875</v>
       </c>
       <c r="I187" s="105"/>
       <c r="J187" s="101"/>
@@ -23526,9 +23530,7 @@
       </c>
       <c r="L187" s="10"/>
       <c r="M187" s="102"/>
-      <c r="N187" s="10" t="s">
-        <v>1483</v>
-      </c>
+      <c r="N187" s="10"/>
       <c r="O187" s="102"/>
       <c r="P187" s="10"/>
       <c r="Q187" s="102"/>
@@ -23540,106 +23542,102 @@
       <c r="W187" s="10"/>
       <c r="X187" s="10"/>
       <c r="Y187" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="Z187" s="10"/>
+    </row>
+    <row r="188" spans="1:27" s="18" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B188" s="23" t="s">
+        <v>1614</v>
+      </c>
+      <c r="C188" s="119" t="str">
+        <f t="shared" si="10"/>
+        <v>EIRD.LPC018c</v>
+      </c>
+      <c r="D188" s="16" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E188" s="23" t="s">
+        <v>398</v>
+      </c>
+      <c r="F188" s="17"/>
+      <c r="G188" s="17"/>
+      <c r="H188" s="116" t="b">
+        <v>1</v>
+      </c>
+      <c r="I188" s="105"/>
+      <c r="J188" s="101"/>
+      <c r="K188" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="L188" s="10"/>
+      <c r="M188" s="102"/>
+      <c r="N188" s="10" t="s">
+        <v>1483</v>
+      </c>
+      <c r="O188" s="102"/>
+      <c r="P188" s="10"/>
+      <c r="Q188" s="102"/>
+      <c r="R188" s="10"/>
+      <c r="S188" s="102"/>
+      <c r="T188" s="10"/>
+      <c r="U188" s="102"/>
+      <c r="V188" s="10"/>
+      <c r="W188" s="10"/>
+      <c r="X188" s="10"/>
+      <c r="Y188" s="16" t="s">
         <v>393</v>
       </c>
-      <c r="Z187" s="10"/>
-    </row>
-    <row r="188" spans="1:27" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B188" s="125"/>
-      <c r="C188" s="125"/>
-      <c r="D188" s="125" t="s">
+      <c r="Z188" s="10"/>
+    </row>
+    <row r="189" spans="1:27" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B189" s="125"/>
+      <c r="C189" s="125"/>
+      <c r="D189" s="125" t="s">
         <v>1412</v>
       </c>
-      <c r="E188" s="125"/>
-      <c r="F188" s="125"/>
-      <c r="G188" s="125"/>
-      <c r="H188" s="125"/>
-      <c r="I188" s="125"/>
-      <c r="J188" s="125"/>
-      <c r="K188" s="125"/>
-      <c r="L188" s="125"/>
-      <c r="M188" s="125"/>
-      <c r="N188" s="125"/>
-      <c r="O188" s="125"/>
-      <c r="P188" s="125"/>
-      <c r="Q188" s="125"/>
-      <c r="R188" s="125"/>
-      <c r="S188" s="125"/>
-      <c r="T188" s="125"/>
-      <c r="U188" s="125"/>
-      <c r="V188" s="125"/>
-      <c r="W188" s="125"/>
-      <c r="X188" s="125"/>
-      <c r="Y188" s="125"/>
-      <c r="Z188" s="125"/>
-    </row>
-    <row r="189" spans="1:27" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="B189" s="23" t="s">
+      <c r="E189" s="125"/>
+      <c r="F189" s="125"/>
+      <c r="G189" s="125"/>
+      <c r="H189" s="125"/>
+      <c r="I189" s="125"/>
+      <c r="J189" s="125"/>
+      <c r="K189" s="125"/>
+      <c r="L189" s="125"/>
+      <c r="M189" s="125"/>
+      <c r="N189" s="125"/>
+      <c r="O189" s="125"/>
+      <c r="P189" s="125"/>
+      <c r="Q189" s="125"/>
+      <c r="R189" s="125"/>
+      <c r="S189" s="125"/>
+      <c r="T189" s="125"/>
+      <c r="U189" s="125"/>
+      <c r="V189" s="125"/>
+      <c r="W189" s="125"/>
+      <c r="X189" s="125"/>
+      <c r="Y189" s="125"/>
+      <c r="Z189" s="125"/>
+    </row>
+    <row r="190" spans="1:27" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="B190" s="23" t="s">
         <v>403</v>
       </c>
-      <c r="C189" s="64" t="s">
+      <c r="C190" s="64" t="s">
         <v>1413</v>
       </c>
-      <c r="D189" s="126" t="s">
+      <c r="D190" s="126" t="s">
         <v>1547</v>
       </c>
-      <c r="E189" s="23" t="s">
+      <c r="E190" s="23" t="s">
         <v>132</v>
-      </c>
-      <c r="F189" s="17"/>
-      <c r="G189" s="17"/>
-      <c r="H189" s="121">
-        <v>44301</v>
-      </c>
-      <c r="I189" s="121"/>
-      <c r="J189" s="105"/>
-      <c r="K189" s="102" t="s">
-        <v>133</v>
-      </c>
-      <c r="L189" s="23" t="s">
-        <v>1271</v>
-      </c>
-      <c r="M189" s="102" t="b">
-        <f ca="1">H189&lt;=TODAY()</f>
-        <v>0</v>
-      </c>
-      <c r="N189" s="10" t="s">
-        <v>1414</v>
-      </c>
-      <c r="O189" s="102"/>
-      <c r="P189" s="10"/>
-      <c r="Q189" s="101"/>
-      <c r="R189" s="10"/>
-      <c r="S189" s="101"/>
-      <c r="T189" s="10"/>
-      <c r="U189" s="101"/>
-      <c r="V189" s="10"/>
-      <c r="W189" s="10"/>
-      <c r="X189" s="10"/>
-      <c r="Y189" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="Z189" s="10"/>
-    </row>
-    <row r="190" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B190" s="23" t="s">
-        <v>404</v>
-      </c>
-      <c r="C190" s="64" t="s">
-        <v>1415</v>
-      </c>
-      <c r="D190" s="126" t="s">
-        <v>1416</v>
-      </c>
-      <c r="E190" s="23" t="s">
-        <v>140</v>
       </c>
       <c r="F190" s="17"/>
       <c r="G190" s="17"/>
-      <c r="H190" s="100" t="s">
-        <v>1417</v>
-      </c>
-      <c r="I190" s="100"/>
+      <c r="H190" s="121">
+        <v>44301</v>
+      </c>
+      <c r="I190" s="121"/>
       <c r="J190" s="105"/>
       <c r="K190" s="102" t="s">
         <v>133</v>
@@ -23647,10 +23645,15 @@
       <c r="L190" s="23" t="s">
         <v>1271</v>
       </c>
-      <c r="M190" s="101"/>
-      <c r="N190" s="23"/>
-      <c r="O190" s="101"/>
-      <c r="P190" s="16"/>
+      <c r="M190" s="102" t="b">
+        <f ca="1">H190&lt;=TODAY()</f>
+        <v>0</v>
+      </c>
+      <c r="N190" s="10" t="s">
+        <v>1414</v>
+      </c>
+      <c r="O190" s="102"/>
+      <c r="P190" s="10"/>
       <c r="Q190" s="101"/>
       <c r="R190" s="10"/>
       <c r="S190" s="101"/>
@@ -23660,27 +23663,27 @@
       <c r="W190" s="10"/>
       <c r="X190" s="10"/>
       <c r="Y190" s="10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Z190" s="10"/>
     </row>
-    <row r="191" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B191" s="23" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C191" s="64" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
       <c r="D191" s="126" t="s">
-        <v>402</v>
+        <v>1416</v>
       </c>
       <c r="E191" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F191" s="23"/>
-      <c r="G191" s="23"/>
+      <c r="F191" s="17"/>
+      <c r="G191" s="17"/>
       <c r="H191" s="100" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="I191" s="100"/>
       <c r="J191" s="105"/>
@@ -23703,30 +23706,36 @@
       <c r="W191" s="10"/>
       <c r="X191" s="10"/>
       <c r="Y191" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Z191" s="10"/>
     </row>
-    <row r="192" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B192" s="23" t="s">
         <v>405</v>
       </c>
       <c r="C192" s="64" t="s">
-        <v>1595</v>
+        <v>1418</v>
       </c>
       <c r="D192" s="126" t="s">
-        <v>1596</v>
+        <v>402</v>
       </c>
       <c r="E192" s="23" t="s">
-        <v>1597</v>
+        <v>140</v>
       </c>
       <c r="F192" s="23"/>
       <c r="G192" s="23"/>
-      <c r="H192" s="100"/>
+      <c r="H192" s="100" t="s">
+        <v>1419</v>
+      </c>
       <c r="I192" s="100"/>
       <c r="J192" s="105"/>
-      <c r="K192" s="102"/>
-      <c r="L192" s="23"/>
+      <c r="K192" s="102" t="s">
+        <v>133</v>
+      </c>
+      <c r="L192" s="23" t="s">
+        <v>1271</v>
+      </c>
       <c r="M192" s="101"/>
       <c r="N192" s="23"/>
       <c r="O192" s="101"/>
@@ -23737,96 +23746,94 @@
       <c r="T192" s="10"/>
       <c r="U192" s="101"/>
       <c r="V192" s="10"/>
-      <c r="W192" s="187"/>
-      <c r="X192" s="187"/>
-      <c r="Y192" s="187"/>
-      <c r="Z192" s="187"/>
-    </row>
-    <row r="193" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B193" s="127"/>
-      <c r="C193" s="24"/>
-      <c r="D193" s="19" t="s">
+      <c r="W192" s="10"/>
+      <c r="X192" s="10"/>
+      <c r="Y192" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="Z192" s="10"/>
+    </row>
+    <row r="193" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B193" s="23" t="s">
+        <v>405</v>
+      </c>
+      <c r="C193" s="64" t="s">
+        <v>1595</v>
+      </c>
+      <c r="D193" s="126" t="s">
+        <v>1596</v>
+      </c>
+      <c r="E193" s="23" t="s">
+        <v>1597</v>
+      </c>
+      <c r="F193" s="23"/>
+      <c r="G193" s="23"/>
+      <c r="H193" s="100"/>
+      <c r="I193" s="100"/>
+      <c r="J193" s="105"/>
+      <c r="K193" s="102"/>
+      <c r="L193" s="23"/>
+      <c r="M193" s="101"/>
+      <c r="N193" s="23"/>
+      <c r="O193" s="101"/>
+      <c r="P193" s="16"/>
+      <c r="Q193" s="101"/>
+      <c r="R193" s="10"/>
+      <c r="S193" s="101"/>
+      <c r="T193" s="10"/>
+      <c r="U193" s="101"/>
+      <c r="V193" s="10"/>
+      <c r="W193" s="187"/>
+      <c r="X193" s="187"/>
+      <c r="Y193" s="187"/>
+      <c r="Z193" s="187"/>
+    </row>
+    <row r="194" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B194" s="127"/>
+      <c r="C194" s="24"/>
+      <c r="D194" s="19" t="s">
         <v>1420</v>
       </c>
-      <c r="E193" s="12"/>
-      <c r="F193" s="12"/>
-      <c r="G193" s="12"/>
-      <c r="H193" s="128"/>
-      <c r="I193" s="128"/>
-      <c r="J193" s="128"/>
-      <c r="K193" s="128"/>
-      <c r="L193" s="128"/>
-      <c r="M193" s="128"/>
-      <c r="N193" s="128"/>
-      <c r="O193" s="128"/>
-      <c r="P193" s="128"/>
-      <c r="Q193" s="128"/>
-      <c r="R193" s="128"/>
-      <c r="S193" s="128"/>
-      <c r="T193" s="128"/>
-      <c r="U193" s="128"/>
-      <c r="V193" s="128"/>
-      <c r="W193" s="165"/>
-      <c r="X193" s="165"/>
-    </row>
-    <row r="194" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B194" s="129" t="s">
+      <c r="E194" s="12"/>
+      <c r="F194" s="12"/>
+      <c r="G194" s="12"/>
+      <c r="H194" s="128"/>
+      <c r="I194" s="128"/>
+      <c r="J194" s="128"/>
+      <c r="K194" s="128"/>
+      <c r="L194" s="128"/>
+      <c r="M194" s="128"/>
+      <c r="N194" s="128"/>
+      <c r="O194" s="128"/>
+      <c r="P194" s="128"/>
+      <c r="Q194" s="128"/>
+      <c r="R194" s="128"/>
+      <c r="S194" s="128"/>
+      <c r="T194" s="128"/>
+      <c r="U194" s="128"/>
+      <c r="V194" s="128"/>
+      <c r="W194" s="165"/>
+      <c r="X194" s="165"/>
+    </row>
+    <row r="195" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B195" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="C194" s="130" t="s">
+      <c r="C195" s="130" t="s">
         <v>1421</v>
       </c>
-      <c r="D194" s="130" t="s">
+      <c r="D195" s="130" t="s">
         <v>1422</v>
       </c>
-      <c r="E194" s="129" t="s">
+      <c r="E195" s="129" t="s">
         <v>1423</v>
       </c>
-      <c r="F194" s="129" t="s">
+      <c r="F195" s="129" t="s">
         <v>1424</v>
-      </c>
-      <c r="G194" s="130"/>
-      <c r="H194" s="101" t="s">
-        <v>1425</v>
-      </c>
-      <c r="I194" s="101"/>
-      <c r="J194" s="101"/>
-      <c r="K194" s="102" t="s">
-        <v>133</v>
-      </c>
-      <c r="L194" s="131"/>
-      <c r="M194" s="101"/>
-      <c r="N194" s="132"/>
-      <c r="O194" s="101"/>
-      <c r="P194" s="129"/>
-      <c r="Q194" s="101"/>
-      <c r="R194" s="129"/>
-      <c r="S194" s="101"/>
-      <c r="T194" s="129"/>
-      <c r="U194" s="101"/>
-      <c r="V194" s="129"/>
-      <c r="W194" s="166"/>
-      <c r="X194" s="166"/>
-    </row>
-    <row r="195" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B195" s="129" t="s">
-        <v>20</v>
-      </c>
-      <c r="C195" s="130" t="s">
-        <v>1426</v>
-      </c>
-      <c r="D195" s="130" t="s">
-        <v>1427</v>
-      </c>
-      <c r="E195" s="129" t="s">
-        <v>1428</v>
-      </c>
-      <c r="F195" s="129" t="s">
-        <v>1268</v>
       </c>
       <c r="G195" s="130"/>
       <c r="H195" s="101" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
       <c r="I195" s="101"/>
       <c r="J195" s="101"/>
@@ -23847,15 +23854,15 @@
       <c r="W195" s="166"/>
       <c r="X195" s="166"/>
     </row>
-    <row r="196" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B196" s="129" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C196" s="130" t="s">
-        <v>1430</v>
+        <v>1426</v>
       </c>
       <c r="D196" s="130" t="s">
-        <v>1031</v>
+        <v>1427</v>
       </c>
       <c r="E196" s="129" t="s">
         <v>1428</v>
@@ -23865,7 +23872,7 @@
       </c>
       <c r="G196" s="130"/>
       <c r="H196" s="101" t="s">
-        <v>1269</v>
+        <v>1429</v>
       </c>
       <c r="I196" s="101"/>
       <c r="J196" s="101"/>
@@ -23886,25 +23893,25 @@
       <c r="W196" s="166"/>
       <c r="X196" s="166"/>
     </row>
-    <row r="197" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B197" s="129" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C197" s="130" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="D197" s="130" t="s">
-        <v>1432</v>
+        <v>1031</v>
       </c>
       <c r="E197" s="129" t="s">
-        <v>1433</v>
+        <v>1428</v>
       </c>
       <c r="F197" s="129" t="s">
-        <v>1424</v>
+        <v>1268</v>
       </c>
       <c r="G197" s="130"/>
-      <c r="H197" s="121">
-        <v>44287</v>
+      <c r="H197" s="101" t="s">
+        <v>1269</v>
       </c>
       <c r="I197" s="101"/>
       <c r="J197" s="101"/>
@@ -23925,15 +23932,15 @@
       <c r="W197" s="166"/>
       <c r="X197" s="166"/>
     </row>
-    <row r="198" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B198" s="129" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C198" s="130" t="s">
-        <v>1434</v>
+        <v>1431</v>
       </c>
       <c r="D198" s="130" t="s">
-        <v>1435</v>
+        <v>1432</v>
       </c>
       <c r="E198" s="129" t="s">
         <v>1433</v>
@@ -23943,7 +23950,7 @@
       </c>
       <c r="G198" s="130"/>
       <c r="H198" s="121">
-        <v>44651</v>
+        <v>44287</v>
       </c>
       <c r="I198" s="101"/>
       <c r="J198" s="101"/>
@@ -23964,30 +23971,30 @@
       <c r="W198" s="166"/>
       <c r="X198" s="166"/>
     </row>
-    <row r="199" spans="2:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B199" s="129" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C199" s="130" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="D199" s="130" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="E199" s="129" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
       <c r="F199" s="129" t="s">
         <v>1424</v>
       </c>
       <c r="G199" s="130"/>
-      <c r="H199" s="101" t="s">
-        <v>1439</v>
+      <c r="H199" s="121">
+        <v>44651</v>
       </c>
       <c r="I199" s="101"/>
       <c r="J199" s="101"/>
       <c r="K199" s="102" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L199" s="131"/>
       <c r="M199" s="101"/>
@@ -24003,30 +24010,30 @@
       <c r="W199" s="166"/>
       <c r="X199" s="166"/>
     </row>
-    <row r="200" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B200" s="129" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C200" s="130" t="s">
-        <v>1440</v>
+        <v>1436</v>
       </c>
       <c r="D200" s="130" t="s">
-        <v>1441</v>
+        <v>1437</v>
       </c>
       <c r="E200" s="129" t="s">
-        <v>1442</v>
+        <v>1438</v>
       </c>
       <c r="F200" s="129" t="s">
         <v>1424</v>
       </c>
       <c r="G200" s="130"/>
-      <c r="H200" s="99">
-        <v>1</v>
+      <c r="H200" s="101" t="s">
+        <v>1439</v>
       </c>
       <c r="I200" s="101"/>
       <c r="J200" s="101"/>
       <c r="K200" s="102" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L200" s="131"/>
       <c r="M200" s="101"/>
@@ -24042,15 +24049,15 @@
       <c r="W200" s="166"/>
       <c r="X200" s="166"/>
     </row>
-    <row r="201" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B201" s="129" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C201" s="130" t="s">
-        <v>1443</v>
+        <v>1440</v>
       </c>
       <c r="D201" s="130" t="s">
-        <v>1444</v>
+        <v>1441</v>
       </c>
       <c r="E201" s="129" t="s">
         <v>1442</v>
@@ -24060,7 +24067,7 @@
       </c>
       <c r="G201" s="130"/>
       <c r="H201" s="99">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I201" s="101"/>
       <c r="J201" s="101"/>
@@ -24081,15 +24088,15 @@
       <c r="W201" s="166"/>
       <c r="X201" s="166"/>
     </row>
-    <row r="202" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B202" s="129" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C202" s="130" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="D202" s="130" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="E202" s="129" t="s">
         <v>1442</v>
@@ -24099,9 +24106,9 @@
       </c>
       <c r="G202" s="130"/>
       <c r="H202" s="99">
-        <v>2</v>
-      </c>
-      <c r="I202" s="99"/>
+        <v>12</v>
+      </c>
+      <c r="I202" s="101"/>
       <c r="J202" s="101"/>
       <c r="K202" s="102" t="s">
         <v>133</v>
@@ -24120,27 +24127,27 @@
       <c r="W202" s="166"/>
       <c r="X202" s="166"/>
     </row>
-    <row r="203" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B203" s="129" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C203" s="130" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="D203" s="130" t="s">
-        <v>1450</v>
+        <v>1446</v>
       </c>
       <c r="E203" s="129" t="s">
-        <v>1485</v>
+        <v>1442</v>
       </c>
       <c r="F203" s="129" t="s">
         <v>1424</v>
       </c>
       <c r="G203" s="130"/>
       <c r="H203" s="99">
-        <v>1</v>
-      </c>
-      <c r="I203" s="101"/>
+        <v>2</v>
+      </c>
+      <c r="I203" s="99"/>
       <c r="J203" s="101"/>
       <c r="K203" s="102" t="s">
         <v>133</v>
@@ -24159,30 +24166,31 @@
       <c r="W203" s="166"/>
       <c r="X203" s="166"/>
     </row>
-    <row r="204" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B204" s="129" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C204" s="130" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="D204" s="130" t="s">
-        <v>1448</v>
+        <v>1450</v>
       </c>
       <c r="E204" s="129" t="s">
-        <v>1442</v>
+        <v>1485</v>
       </c>
       <c r="F204" s="129" t="s">
         <v>1424</v>
       </c>
       <c r="G204" s="130"/>
       <c r="H204" s="99">
-        <f>18264</f>
-        <v>18264</v>
-      </c>
-      <c r="I204" s="99"/>
+        <v>1</v>
+      </c>
+      <c r="I204" s="101"/>
       <c r="J204" s="101"/>
-      <c r="K204" s="102"/>
+      <c r="K204" s="102" t="s">
+        <v>133</v>
+      </c>
       <c r="L204" s="131"/>
       <c r="M204" s="101"/>
       <c r="N204" s="132"/>
@@ -24197,30 +24205,33 @@
       <c r="W204" s="166"/>
       <c r="X204" s="166"/>
     </row>
-    <row r="205" spans="2:24" ht="318.75" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B205" s="129" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C205" s="130" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="D205" s="130" t="s">
-        <v>1452</v>
+        <v>1448</v>
       </c>
       <c r="E205" s="129" t="s">
-        <v>1453</v>
-      </c>
-      <c r="F205" s="129"/>
+        <v>1442</v>
+      </c>
+      <c r="F205" s="129" t="s">
+        <v>1424</v>
+      </c>
       <c r="G205" s="130"/>
-      <c r="H205" s="121" t="s">
-        <v>1454</v>
-      </c>
-      <c r="I205" s="121"/>
+      <c r="H205" s="99">
+        <f>18264</f>
+        <v>18264</v>
+      </c>
+      <c r="I205" s="99"/>
       <c r="J205" s="101"/>
-      <c r="K205" s="101"/>
-      <c r="L205" s="133"/>
+      <c r="K205" s="102"/>
+      <c r="L205" s="131"/>
       <c r="M205" s="101"/>
-      <c r="N205" s="134"/>
+      <c r="N205" s="132"/>
       <c r="O205" s="101"/>
       <c r="P205" s="129"/>
       <c r="Q205" s="101"/>
@@ -24232,15 +24243,15 @@
       <c r="W205" s="166"/>
       <c r="X205" s="166"/>
     </row>
-    <row r="206" spans="2:24" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:26" ht="318.75" x14ac:dyDescent="0.2">
       <c r="B206" s="129" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C206" s="130" t="s">
-        <v>1455</v>
+        <v>1451</v>
       </c>
       <c r="D206" s="130" t="s">
-        <v>1456</v>
+        <v>1452</v>
       </c>
       <c r="E206" s="129" t="s">
         <v>1453</v>
@@ -24248,7 +24259,7 @@
       <c r="F206" s="129"/>
       <c r="G206" s="130"/>
       <c r="H206" s="121" t="s">
-        <v>1545</v>
+        <v>1454</v>
       </c>
       <c r="I206" s="121"/>
       <c r="J206" s="101"/>
@@ -24267,15 +24278,15 @@
       <c r="W206" s="166"/>
       <c r="X206" s="166"/>
     </row>
-    <row r="207" spans="2:24" ht="357" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:26" ht="409.5" x14ac:dyDescent="0.2">
       <c r="B207" s="129" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C207" s="130" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="D207" s="130" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="E207" s="129" t="s">
         <v>1453</v>
@@ -24283,7 +24294,7 @@
       <c r="F207" s="129"/>
       <c r="G207" s="130"/>
       <c r="H207" s="121" t="s">
-        <v>1459</v>
+        <v>1545</v>
       </c>
       <c r="I207" s="121"/>
       <c r="J207" s="101"/>
@@ -24302,25 +24313,25 @@
       <c r="W207" s="166"/>
       <c r="X207" s="166"/>
     </row>
-    <row r="208" spans="2:24" ht="229.5" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:26" ht="357" x14ac:dyDescent="0.2">
       <c r="B208" s="129" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C208" s="130" t="s">
-        <v>1460</v>
+        <v>1457</v>
       </c>
       <c r="D208" s="130" t="s">
-        <v>1461</v>
+        <v>1458</v>
       </c>
       <c r="E208" s="129" t="s">
         <v>1453</v>
       </c>
       <c r="F208" s="129"/>
       <c r="G208" s="130"/>
-      <c r="H208" s="101" t="s">
-        <v>1546</v>
-      </c>
-      <c r="I208" s="101"/>
+      <c r="H208" s="121" t="s">
+        <v>1459</v>
+      </c>
+      <c r="I208" s="121"/>
       <c r="J208" s="101"/>
       <c r="K208" s="101"/>
       <c r="L208" s="133"/>
@@ -24337,8 +24348,43 @@
       <c r="W208" s="166"/>
       <c r="X208" s="166"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B209" s="167" t="s">
+    <row r="209" spans="2:24" ht="229.5" x14ac:dyDescent="0.2">
+      <c r="B209" s="129" t="s">
+        <v>33</v>
+      </c>
+      <c r="C209" s="130" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D209" s="130" t="s">
+        <v>1461</v>
+      </c>
+      <c r="E209" s="129" t="s">
+        <v>1453</v>
+      </c>
+      <c r="F209" s="129"/>
+      <c r="G209" s="130"/>
+      <c r="H209" s="101" t="s">
+        <v>1546</v>
+      </c>
+      <c r="I209" s="101"/>
+      <c r="J209" s="101"/>
+      <c r="K209" s="101"/>
+      <c r="L209" s="133"/>
+      <c r="M209" s="101"/>
+      <c r="N209" s="134"/>
+      <c r="O209" s="101"/>
+      <c r="P209" s="129"/>
+      <c r="Q209" s="101"/>
+      <c r="R209" s="129"/>
+      <c r="S209" s="101"/>
+      <c r="T209" s="129"/>
+      <c r="U209" s="101"/>
+      <c r="V209" s="129"/>
+      <c r="W209" s="166"/>
+      <c r="X209" s="166"/>
+    </row>
+    <row r="210" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B210" s="167" t="s">
         <v>1567</v>
       </c>
     </row>
@@ -24359,7 +24405,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z126" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>FacUndrawnFor</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Determine naming convention" sqref="K189:K192 M188 E188:E192 M190:M192 B194:B208 B189:B192" xr:uid="{00000000-0002-0000-0200-000005000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Determine naming convention" sqref="K190:K193 M189 E189:E193 M191:M193 B195:B209 B190:B193" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -24402,14 +24448,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z16" xr:uid="{00000000-0002-0000-0200-000012000000}">
       <formula1>"accountyear"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Determine naming convention" sqref="C104:C110 A102:A110 D53 C8:C101 C178:C187 C112:C135 B8:B187 C137:C176" xr:uid="{00000000-0002-0000-0200-000013000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z105 Z171" xr:uid="{00000000-0002-0000-0200-000014000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Determine naming convention" sqref="C104:C110 A102:A110 D53 C179:C188 C112:C135 C137:C177 C8:C101 B8:B188" xr:uid="{00000000-0002-0000-0200-000013000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z105 Z172" xr:uid="{00000000-0002-0000-0200-000014000000}">
       <formula1>TypeofCove</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z108 Z174" xr:uid="{00000000-0002-0000-0200-000015000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z108 Z175" xr:uid="{00000000-0002-0000-0200-000015000000}">
       <formula1>FreqReportCove</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z181" xr:uid="{00000000-0002-0000-0200-000016000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z182" xr:uid="{00000000-0002-0000-0200-000016000000}">
       <formula1>IRDType</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
FYFP and Stock updates
</commit_message>
<xml_diff>
--- a/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.3.xlsx
+++ b/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ShrForms\specifications\lp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC310A1-CE8C-42B2-AE86-A28DBC079F58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB38F30B-1F25-49ED-9B97-7D396658DF8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="804" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5235,9 +5235,6 @@
     <t>LPC101</t>
   </si>
   <si>
-    <t>Grid({"page":"loancovenant", "createLabel":"Create Loan Covenant", "columns":[]})</t>
-  </si>
-  <si>
     <t>EIRD</t>
   </si>
   <si>
@@ -5267,7 +5264,10 @@
     <t>Loan Covenants</t>
   </si>
   <si>
-    <t>Select({"page":"loancovenant", "createLabel":"Add existing Loan Covenant", "title":"Select Loan Covenants", "useParent": true, "columns":["lpc004"]})</t>
+    <t>Select({"page":"loancovenant", "createLabel":"Manage Linked Loan Covenants", "title":"Loan Covenants", "useParent": true, "columns":["lpc004", "lpc005", "lpc007"]})</t>
+  </si>
+  <si>
+    <t>Grid({"page":"loancovenant", "createLabel":"Create Loan Covenant", "columns":["lpc004","lpc005", "lpc007"]})</t>
   </si>
 </sst>
 </file>
@@ -14580,10 +14580,10 @@
       </c>
       <c r="B12" s="39"/>
       <c r="C12" s="33" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="F12" s="39" t="s">
         <v>1027</v>
@@ -15193,8 +15193,8 @@
   <dimension ref="A1:AA210"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD26"/>
+      <pane ySplit="8" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15446,7 +15446,7 @@
       </c>
       <c r="I11" s="107"/>
       <c r="J11" s="101" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="K11" s="108" t="s">
         <v>135</v>
@@ -21048,7 +21048,7 @@
       <c r="D134" s="180" t="s">
         <v>1052</v>
       </c>
-      <c r="E134" s="182" t="s">
+      <c r="E134" s="181" t="s">
         <v>1605</v>
       </c>
       <c r="F134" s="183"/>
@@ -21085,8 +21085,8 @@
       <c r="D135" s="180" t="s">
         <v>1020</v>
       </c>
-      <c r="E135" s="182" t="s">
-        <v>1608</v>
+      <c r="E135" s="181" t="s">
+        <v>1618</v>
       </c>
       <c r="F135" s="183"/>
       <c r="G135" s="183"/>
@@ -22628,17 +22628,17 @@
     <row r="167" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="15"/>
       <c r="B167" s="179" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="C167" s="119" t="str">
         <f t="shared" si="8"/>
         <v>Loan.LPL100</v>
       </c>
       <c r="D167" s="180" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E167" s="181" t="s">
         <v>1612</v>
-      </c>
-      <c r="E167" s="182" t="s">
-        <v>1613</v>
       </c>
       <c r="F167" s="183"/>
       <c r="G167" s="183"/>
@@ -22665,17 +22665,17 @@
     <row r="168" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="15"/>
       <c r="B168" s="179" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="C168" s="119" t="str">
         <f t="shared" si="8"/>
         <v>Loan.LPL101</v>
       </c>
       <c r="D168" s="180" t="s">
+        <v>1616</v>
+      </c>
+      <c r="E168" s="181" t="s">
         <v>1617</v>
-      </c>
-      <c r="E168" s="182" t="s">
-        <v>1618</v>
       </c>
       <c r="F168" s="183"/>
       <c r="G168" s="183"/>
@@ -23292,7 +23292,7 @@
         <v>1534</v>
       </c>
       <c r="E182" s="23" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="F182" s="17"/>
       <c r="G182" s="17"/>
@@ -23548,7 +23548,7 @@
     </row>
     <row r="188" spans="1:27" s="18" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B188" s="23" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="C188" s="119" t="str">
         <f t="shared" si="10"/>
@@ -25786,7 +25786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0"/>
+    <sheetView topLeftCell="A31" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
LP WIP - Including ISDA
</commit_message>
<xml_diff>
--- a/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.3.xlsx
+++ b/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ShrForms\specifications\lp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2F0569-02DF-4C2F-8504-238F4D34FF5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4258D0E9-214C-4C89-AD54-74A07A867A3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="804" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2697" uniqueCount="1638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2694" uniqueCount="1639">
   <si>
     <t>Field ID</t>
   </si>
@@ -4927,10 +4927,6 @@
   </si>
   <si>
     <t>DERIVED
-ISDA Covenant counter + 1</t>
-  </si>
-  <si>
-    <t>DERIVED
 Loan Covenant counter + 1</t>
   </si>
   <si>
@@ -5326,6 +5322,12 @@
   </si>
   <si>
     <t>MultiChoice(lender.csv)</t>
+  </si>
+  <si>
+    <t>LPC025a</t>
+  </si>
+  <si>
+    <t>Choice(isda_frequency_call.csv)</t>
   </si>
 </sst>
 </file>
@@ -8389,7 +8391,7 @@
         <v>1010</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
   </sheetData>
@@ -8740,7 +8742,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B70" s="44" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -8781,7 +8783,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -8827,7 +8829,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
   </sheetData>
@@ -8864,7 +8866,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="B3" s="140" t="e">
         <f>Data!I168</f>
@@ -8968,7 +8970,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="B3" s="140" t="e">
         <f>Data!#REF!</f>
@@ -8995,7 +8997,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="44" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="B9" t="str">
         <f>Data!H179</f>
@@ -9016,7 +9018,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="44" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="B13" s="112">
         <f>Data!H181</f>
@@ -9025,7 +9027,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="44" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="B15" s="112">
         <f>Data!H182</f>
@@ -9034,7 +9036,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="44" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="B17">
         <f>Data!H183</f>
@@ -9043,7 +9045,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="44" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="B19">
         <f>Data!H184</f>
@@ -9052,7 +9054,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="44" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="B21" t="b">
         <f>Data!H185</f>
@@ -14231,16 +14233,16 @@
         <v>349</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>350</v>
       </c>
       <c r="D1" s="31" t="s">
+        <v>1558</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>1559</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>1560</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>148</v>
@@ -14493,18 +14495,18 @@
     </row>
     <row r="2" spans="1:251" x14ac:dyDescent="0.2">
       <c r="A2" s="89" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="B2" s="89"/>
       <c r="C2" s="89" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="D2" s="89"/>
       <c r="E2" s="89" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="3" spans="1:251" x14ac:dyDescent="0.2">
@@ -14525,18 +14527,18 @@
     </row>
     <row r="4" spans="1:251" x14ac:dyDescent="0.2">
       <c r="A4" s="89" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="B4" s="89"/>
       <c r="C4" s="89" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="D4" s="89"/>
       <c r="E4" s="89" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="5" spans="1:251" x14ac:dyDescent="0.2">
@@ -14545,14 +14547,14 @@
       </c>
       <c r="B5" s="39"/>
       <c r="C5" s="33" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="33" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="6" spans="1:251" x14ac:dyDescent="0.2">
@@ -14561,14 +14563,14 @@
       </c>
       <c r="B6" s="39"/>
       <c r="C6" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="D6" s="33"/>
       <c r="E6" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="7" spans="1:251" x14ac:dyDescent="0.2">
@@ -14593,11 +14595,11 @@
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="33" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="D8" s="33"/>
       <c r="E8" s="33" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="F8" s="34" t="s">
         <v>1011</v>
@@ -14641,11 +14643,11 @@
       </c>
       <c r="B11" s="39"/>
       <c r="C11" s="89" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="89" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="F11" s="89" t="s">
         <v>1014</v>
@@ -14657,10 +14659,10 @@
       </c>
       <c r="B12" s="39"/>
       <c r="C12" s="33" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="F12" s="39" t="s">
         <v>1021</v>
@@ -15253,7 +15255,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -15270,8 +15272,8 @@
   <dimension ref="A1:AA210"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A141" sqref="A141"/>
+      <pane ySplit="8" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15308,14 +15310,14 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B2" s="157" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="C2" s="158"/>
       <c r="D2" s="156"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B3" s="159" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="C3" s="159"/>
       <c r="D3" s="160"/>
@@ -15325,12 +15327,12 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B4" s="159" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="C4" s="159"/>
       <c r="D4" s="161"/>
       <c r="G4" s="205" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -15402,22 +15404,22 @@
         <v>1329</v>
       </c>
       <c r="S8" s="11" t="s">
+        <v>1538</v>
+      </c>
+      <c r="T8" s="11" t="s">
         <v>1539</v>
       </c>
-      <c r="T8" s="11" t="s">
+      <c r="U8" s="11" t="s">
         <v>1540</v>
       </c>
-      <c r="U8" s="11" t="s">
-        <v>1541</v>
-      </c>
       <c r="V8" s="11" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="W8" s="11" t="s">
+        <v>1554</v>
+      </c>
+      <c r="X8" s="11" t="s">
         <v>1555</v>
-      </c>
-      <c r="X8" s="11" t="s">
-        <v>1556</v>
       </c>
       <c r="Y8" s="11" t="s">
         <v>140</v>
@@ -15526,7 +15528,7 @@
       </c>
       <c r="I11" s="107"/>
       <c r="J11" s="101" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="K11" s="108" t="s">
         <v>133</v>
@@ -15610,7 +15612,7 @@
         <v>Submission.LPR005</v>
       </c>
       <c r="D13" s="109" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="E13" s="108" t="s">
         <v>130</v>
@@ -15655,7 +15657,7 @@
         <v>Submission.LPR005a</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>130</v>
@@ -16016,7 +16018,7 @@
     <row r="22" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
       <c r="B22" s="179" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="C22" s="179" t="str">
         <f>"Submission." &amp; B22</f>
@@ -16026,7 +16028,7 @@
         <v>1012</v>
       </c>
       <c r="E22" s="181" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="F22" s="183"/>
       <c r="G22" s="183"/>
@@ -16053,7 +16055,7 @@
     <row r="23" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
       <c r="B23" s="179" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="C23" s="179" t="str">
         <f t="shared" ref="C23" si="1">"Submission." &amp; B23</f>
@@ -16063,7 +16065,7 @@
         <v>896</v>
       </c>
       <c r="E23" s="181" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="F23" s="183"/>
       <c r="G23" s="183"/>
@@ -16090,17 +16092,17 @@
     <row r="24" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
       <c r="B24" s="179" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="C24" s="179" t="str">
         <f t="shared" si="0"/>
         <v>Submission.LPR100</v>
       </c>
       <c r="D24" s="180" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="E24" s="182" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="F24" s="183"/>
       <c r="G24" s="183"/>
@@ -16127,17 +16129,17 @@
     <row r="25" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
       <c r="B25" s="179" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="C25" s="179" t="str">
         <f t="shared" ref="C25" si="2">"Submission." &amp; B25</f>
         <v>Submission.LPR101</v>
       </c>
       <c r="D25" s="180" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="E25" s="181" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="F25" s="183"/>
       <c r="G25" s="183"/>
@@ -16674,7 +16676,7 @@
         <v>IGFLend.LPIGF009</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>130</v>
@@ -16720,7 +16722,7 @@
         <v>IGFLend.LPIGF010</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>130</v>
@@ -17674,7 +17676,7 @@
     <row r="59" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="15"/>
       <c r="B59" s="108" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="C59" s="119" t="str">
         <f t="shared" si="4"/>
@@ -18063,7 +18065,7 @@
         <v>IGFBorrow.LPIGF033</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>130</v>
@@ -18109,7 +18111,7 @@
         <v>IGFBorrow.LPIGF034</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="E68" s="9" t="s">
         <v>130</v>
@@ -19127,8 +19129,8 @@
       </c>
       <c r="F90" s="17"/>
       <c r="G90" s="17"/>
-      <c r="H90" s="104" t="s">
-        <v>859</v>
+      <c r="H90" s="104">
+        <v>3</v>
       </c>
       <c r="I90" s="105"/>
       <c r="J90" s="101"/>
@@ -19194,7 +19196,10 @@
       <c r="T91" s="16"/>
       <c r="U91" s="102"/>
       <c r="V91" s="16"/>
-      <c r="W91" s="16"/>
+      <c r="W91" s="16" t="b">
+        <f>H90&lt;&gt;3</f>
+        <v>0</v>
+      </c>
       <c r="X91" s="16"/>
       <c r="Y91" s="16" t="s">
         <v>326</v>
@@ -19203,11 +19208,11 @@
     </row>
     <row r="92" spans="1:26" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="23" t="s">
-        <v>82</v>
+        <v>1637</v>
       </c>
       <c r="C92" s="119" t="str">
         <f t="shared" si="5"/>
-        <v>ISDA.LPC025</v>
+        <v>ISDA.LPC025a</v>
       </c>
       <c r="D92" s="16" t="s">
         <v>1361</v>
@@ -19238,7 +19243,10 @@
       <c r="T92" s="10"/>
       <c r="U92" s="102"/>
       <c r="V92" s="10"/>
-      <c r="W92" s="10"/>
+      <c r="W92" s="16" t="b">
+        <f>H90=3</f>
+        <v>1</v>
+      </c>
       <c r="X92" s="10"/>
       <c r="Y92" s="16" t="s">
         <v>326</v>
@@ -19492,8 +19500,8 @@
       </c>
       <c r="F98" s="17"/>
       <c r="G98" s="17"/>
-      <c r="H98" s="104" t="s">
-        <v>879</v>
+      <c r="H98" s="104">
+        <v>3</v>
       </c>
       <c r="I98" s="105"/>
       <c r="J98" s="101"/>
@@ -19559,7 +19567,10 @@
       <c r="T99" s="10"/>
       <c r="U99" s="102"/>
       <c r="V99" s="10"/>
-      <c r="W99" s="10"/>
+      <c r="W99" s="10" t="b">
+        <f>H98=3</f>
+        <v>1</v>
+      </c>
       <c r="X99" s="10"/>
       <c r="Y99" s="16" t="s">
         <v>332</v>
@@ -19578,7 +19589,7 @@
         <v>185</v>
       </c>
       <c r="E100" s="23" t="s">
-        <v>1365</v>
+        <v>1638</v>
       </c>
       <c r="F100" s="17"/>
       <c r="G100" s="17"/>
@@ -19615,7 +19626,7 @@
     <row r="101" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="15"/>
       <c r="B101" s="179" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="C101" s="186" t="str">
         <f>"ISDA." &amp; B101</f>
@@ -19625,7 +19636,7 @@
         <v>1011</v>
       </c>
       <c r="E101" s="182" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="F101" s="183"/>
       <c r="G101" s="183"/>
@@ -19739,8 +19750,9 @@
         <v>1271</v>
       </c>
       <c r="F104" s="108"/>
-      <c r="G104" s="109" t="s">
-        <v>1513</v>
+      <c r="G104" s="109" t="str">
+        <f>Pfo_Page_Serial_Padded_4</f>
+        <v>0002</v>
       </c>
       <c r="H104" s="103"/>
       <c r="I104" s="107">
@@ -19784,7 +19796,7 @@
         <v>340</v>
       </c>
       <c r="E105" s="23" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="F105" s="17"/>
       <c r="G105" s="17"/>
@@ -19846,7 +19858,7 @@
       <c r="L106" s="10"/>
       <c r="M106" s="102"/>
       <c r="N106" s="10" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="O106" s="102"/>
       <c r="P106" s="10"/>
@@ -20135,7 +20147,7 @@
         <v>Facility.LPF001</v>
       </c>
       <c r="D113" s="16" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="E113" s="23" t="s">
         <v>1357</v>
@@ -20147,7 +20159,7 @@
       </c>
       <c r="I113" s="105"/>
       <c r="J113" s="104" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="K113" s="9" t="s">
         <v>131</v>
@@ -20232,7 +20244,7 @@
         <v>346</v>
       </c>
       <c r="E115" s="23" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="F115" s="17"/>
       <c r="G115" s="17"/>
@@ -20375,7 +20387,7 @@
         <v>1371</v>
       </c>
       <c r="E118" s="23" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="F118" s="17"/>
       <c r="G118" s="17"/>
@@ -20769,7 +20781,7 @@
         <v>408</v>
       </c>
       <c r="E126" s="23" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="F126" s="17"/>
       <c r="G126" s="17"/>
@@ -21126,7 +21138,7 @@
     <row r="134" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="15"/>
       <c r="B134" s="179" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="C134" s="186" t="str">
         <f>"Facility." &amp; B134</f>
@@ -21136,7 +21148,7 @@
         <v>1046</v>
       </c>
       <c r="E134" s="181" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="F134" s="183"/>
       <c r="G134" s="183"/>
@@ -21163,7 +21175,7 @@
     <row r="135" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="15"/>
       <c r="B135" s="179" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="C135" s="186" t="str">
         <f>"Facility." &amp; B135</f>
@@ -21173,7 +21185,7 @@
         <v>1014</v>
       </c>
       <c r="E135" s="181" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="F135" s="183"/>
       <c r="G135" s="183"/>
@@ -21301,7 +21313,7 @@
       </c>
       <c r="M138" s="117"/>
       <c r="N138" s="10" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="O138" s="102"/>
       <c r="P138" s="10"/>
@@ -21697,7 +21709,7 @@
       </c>
       <c r="I146" s="105"/>
       <c r="J146" s="101" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="K146" s="9" t="s">
         <v>131</v>
@@ -21707,28 +21719,28 @@
       </c>
       <c r="M146" s="168"/>
       <c r="N146" s="10" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="O146" s="102" t="b">
         <f>OR(OR(H138="Fixed Rate Loan",H138="Fixed with embedded Interest Rate Swaps",H138="Fixed without embedded Interest Rate Swaps",H138="Bond / Capital Market product",H138="Development Overdraft", H138="Revolving Loan / Credit Facility",LEFT(H138,8)="Variable",H138="Working Capital Overdraft (if &gt; £1m)"),AND(H138="Fixed Interest Free",H146="Interest Free"))</f>
         <v>0</v>
       </c>
       <c r="P146" s="10" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="Q146" s="102" t="b">
         <f>OR(OR(H146="Base",H146="Interest Free",H146="Lenders Mortgage Base Rate",LEFT(H146,5)="LIBOR",H146="Rate paid by on lender (for on lending only)",H146="RPI linked"),AND(H146="Fixed Rate Percentage",H138="Fixed Rate Loan"))</f>
         <v>0</v>
       </c>
       <c r="R146" s="10" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="S146" s="102" t="b">
         <f>OR(OR(H146="Base",H146="Fixed Rate Percentage",H146="Lenders Mortgage Base Rate",LEFT(H146,5)="LIBOR",H146="Rate paid by on lender (for on lending only)",H146="RPI linked"),AND(H146=" Interest Free",H138="Fixed Interest Free"))</f>
         <v>0</v>
       </c>
       <c r="T146" s="10" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="U146" s="102"/>
       <c r="V146" s="10"/>
@@ -21790,7 +21802,7 @@
     </row>
     <row r="148" spans="2:27" ht="116.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B148" s="23" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="C148" s="119" t="str">
         <f t="shared" si="8"/>
@@ -22026,28 +22038,28 @@
         <v>1</v>
       </c>
       <c r="P152" s="10" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="Q152" s="102" t="b">
         <f>OR(OR(H145="Interest only - Bullet repayment at end of term from cashflow",H145="Interest only - Bullet repayment at end of term from refinancing",H145="Interest only then capital and interest",H145="Interest only until fully drawn",H145="Interest only followed by structured capital repayments",H145="Repayable on demand",H145="Converted to loan",H145="Subject to annual renewal"),AND(OR(H145="Fully Amortising",H145="Payment start date deferred then fully amortising", H145="Payment start date deferred-bullet repayment of interest and capital at maturity",H145="Interest &amp; capital then bullet repayment from cashflow or refinancing"),H152=H150))</f>
         <v>0</v>
       </c>
       <c r="R152" s="10" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="S152" s="102" t="b">
         <f>OR(OR(H145="Fully Amortising",H145="Payment start date deferred then fully amortising", H145="Payment start date deferred-bullet repayment of interest and capital at maturity",H145="Interest &amp; capital then bullet repayment from cashflow or refinancing",H145="Interest only - Bullet repayment at end of term from cashflow",H145="Interest only - Bullet repayment at end of term from refinancing", H145="Repayable on demand",H145="Converted to loan",H145="Subject to annual renewal"),AND(OR(H145="Interest only then capital and interest",H145="Interest only until fully drawn",H145="Interest only followed by structured capital repayments",),J152&lt;J150))</f>
         <v>1</v>
       </c>
       <c r="T152" s="10" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="U152" s="102" t="b">
         <f>OR(OR(H145="Fully Amortising",H145="Payment start date deferred then fully amortising", H145="Payment start date deferred-bullet repayment of interest and capital at maturity",H145="Interest &amp; capital then bullet repayment from cashflow or refinancing", H145="Interest only then capital and interest", H145="Interest only followed by structured capital repayments",H145="Repayable on demand",H145="Converted to loan",H145="Subject to annual renewal"),AND(OR(H145="Interest only - Bullet repayment at end of term from cashflow",H145="Interest only - Bullet repayment at end of term from refinancing",H145="Interest only until fully drawn",),L152&lt;L151))</f>
         <v>1</v>
       </c>
       <c r="V152" s="10" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="W152" s="10"/>
       <c r="X152" s="10"/>
@@ -22216,7 +22228,7 @@
         <v>972</v>
       </c>
       <c r="E156" s="23" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="F156" s="17"/>
       <c r="G156" s="17"/>
@@ -22674,17 +22686,17 @@
     <row r="166" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="15"/>
       <c r="B166" s="179" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="C166" s="119" t="str">
         <f t="shared" si="8"/>
         <v>Loan.LPL100</v>
       </c>
       <c r="D166" s="180" t="s">
+        <v>1600</v>
+      </c>
+      <c r="E166" s="181" t="s">
         <v>1601</v>
-      </c>
-      <c r="E166" s="181" t="s">
-        <v>1602</v>
       </c>
       <c r="F166" s="183"/>
       <c r="G166" s="183"/>
@@ -22711,17 +22723,17 @@
     <row r="167" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="15"/>
       <c r="B167" s="179" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="C167" s="119" t="str">
         <f t="shared" si="8"/>
         <v>Loan.LPL101</v>
       </c>
       <c r="D167" s="180" t="s">
+        <v>1605</v>
+      </c>
+      <c r="E167" s="181" t="s">
         <v>1606</v>
-      </c>
-      <c r="E167" s="181" t="s">
-        <v>1607</v>
       </c>
       <c r="F167" s="183"/>
       <c r="G167" s="183"/>
@@ -22858,7 +22870,7 @@
         <v>1262</v>
       </c>
       <c r="G170" s="109" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="H170" s="103"/>
       <c r="I170" s="107">
@@ -22900,7 +22912,7 @@
         <v>340</v>
       </c>
       <c r="E171" s="23" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="F171" s="17"/>
       <c r="G171" s="17"/>
@@ -22949,7 +22961,7 @@
       <c r="F172" s="17"/>
       <c r="G172" s="17"/>
       <c r="H172" s="104" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="I172" s="105"/>
       <c r="J172" s="120"/>
@@ -22959,7 +22971,7 @@
       <c r="L172" s="10"/>
       <c r="M172" s="102"/>
       <c r="N172" s="10" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="O172" s="102"/>
       <c r="P172" s="10"/>
@@ -22993,7 +23005,7 @@
       <c r="F173" s="17"/>
       <c r="G173" s="17"/>
       <c r="H173" s="149" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="I173" s="105"/>
       <c r="J173" s="120"/>
@@ -23125,7 +23137,7 @@
       <c r="F176" s="17"/>
       <c r="G176" s="17"/>
       <c r="H176" s="149" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="I176" s="105"/>
       <c r="J176" s="120"/>
@@ -23201,7 +23213,7 @@
         <v>1262</v>
       </c>
       <c r="G178" s="109" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="H178" s="103"/>
       <c r="I178" s="107">
@@ -23241,10 +23253,10 @@
         <v>EIRD.LPC014</v>
       </c>
       <c r="D179" s="16" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="E179" s="23" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="F179" s="17"/>
       <c r="G179" s="17"/>
@@ -23329,7 +23341,7 @@
         <v>EIRD.LPC016</v>
       </c>
       <c r="D181" s="16" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="E181" s="23" t="s">
         <v>130</v>
@@ -23374,7 +23386,7 @@
         <v>EIRD.LPC017</v>
       </c>
       <c r="D182" s="16" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="E182" s="23" t="s">
         <v>130</v>
@@ -23395,7 +23407,7 @@
         <v>1</v>
       </c>
       <c r="N182" s="10" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="O182" s="102"/>
       <c r="P182" s="10"/>
@@ -23416,14 +23428,14 @@
     </row>
     <row r="183" spans="1:27" s="18" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B183" s="23" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="C183" s="119" t="str">
         <f t="shared" si="10"/>
         <v>EIRD.LPC018a</v>
       </c>
       <c r="D183" s="16" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="E183" s="9" t="s">
         <v>1304</v>
@@ -23465,7 +23477,7 @@
         <v>EIRD.LPC018b</v>
       </c>
       <c r="D184" s="16" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="E184" s="9" t="s">
         <v>1304</v>
@@ -23500,14 +23512,14 @@
     </row>
     <row r="185" spans="1:27" s="18" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B185" s="23" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="C185" s="119" t="str">
         <f t="shared" si="10"/>
         <v>EIRD.LPC018c</v>
       </c>
       <c r="D185" s="16" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E185" s="23" t="s">
         <v>392</v>
@@ -23579,7 +23591,7 @@
         <v>1404</v>
       </c>
       <c r="D187" s="126" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="E187" s="23" t="s">
         <v>130</v>
@@ -23710,13 +23722,13 @@
         <v>399</v>
       </c>
       <c r="C190" s="64" t="s">
+        <v>1584</v>
+      </c>
+      <c r="D190" s="126" t="s">
         <v>1585</v>
       </c>
-      <c r="D190" s="126" t="s">
+      <c r="E190" s="23" t="s">
         <v>1586</v>
-      </c>
-      <c r="E190" s="23" t="s">
-        <v>1587</v>
       </c>
       <c r="F190" s="23"/>
       <c r="G190" s="23"/>
@@ -23769,7 +23781,7 @@
     </row>
     <row r="192" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B192" s="129" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="C192" s="130" t="s">
         <v>1412</v>
@@ -23808,7 +23820,7 @@
     </row>
     <row r="193" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B193" s="129" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="C193" s="130" t="s">
         <v>1417</v>
@@ -23847,7 +23859,7 @@
     </row>
     <row r="194" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B194" s="129" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="C194" s="130" t="s">
         <v>1421</v>
@@ -23886,7 +23898,7 @@
     </row>
     <row r="195" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B195" s="129" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="C195" s="130" t="s">
         <v>1422</v>
@@ -23925,7 +23937,7 @@
     </row>
     <row r="196" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B196" s="129" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="C196" s="130" t="s">
         <v>1425</v>
@@ -23964,7 +23976,7 @@
     </row>
     <row r="197" spans="2:24" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B197" s="129" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="C197" s="130" t="s">
         <v>1427</v>
@@ -24003,7 +24015,7 @@
     </row>
     <row r="198" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B198" s="129" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="C198" s="130" t="s">
         <v>1431</v>
@@ -24042,7 +24054,7 @@
     </row>
     <row r="199" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B199" s="129" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="C199" s="130" t="s">
         <v>1434</v>
@@ -24081,7 +24093,7 @@
     </row>
     <row r="200" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B200" s="129" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C200" s="130" t="s">
         <v>1436</v>
@@ -24120,7 +24132,7 @@
     </row>
     <row r="201" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B201" s="129" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="C201" s="130" t="s">
         <v>1438</v>
@@ -24159,7 +24171,7 @@
     </row>
     <row r="202" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B202" s="129" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="C202" s="130" t="s">
         <v>1440</v>
@@ -24197,7 +24209,7 @@
     </row>
     <row r="203" spans="2:24" ht="318.75" x14ac:dyDescent="0.2">
       <c r="B203" s="129" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="C203" s="130" t="s">
         <v>1442</v>
@@ -24232,7 +24244,7 @@
     </row>
     <row r="204" spans="2:24" ht="409.5" x14ac:dyDescent="0.2">
       <c r="B204" s="129" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="C204" s="130" t="s">
         <v>1446</v>
@@ -24246,7 +24258,7 @@
       <c r="F204" s="129"/>
       <c r="G204" s="130"/>
       <c r="H204" s="121" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="I204" s="121"/>
       <c r="J204" s="101"/>
@@ -24267,7 +24279,7 @@
     </row>
     <row r="205" spans="2:24" ht="357" x14ac:dyDescent="0.2">
       <c r="B205" s="129" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="C205" s="130" t="s">
         <v>1448</v>
@@ -24302,7 +24314,7 @@
     </row>
     <row r="206" spans="2:24" ht="229.5" x14ac:dyDescent="0.2">
       <c r="B206" s="129" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="C206" s="130" t="s">
         <v>1451</v>
@@ -24316,7 +24328,7 @@
       <c r="F206" s="129"/>
       <c r="G206" s="130"/>
       <c r="H206" s="101" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="I206" s="101"/>
       <c r="J206" s="101"/>
@@ -24337,13 +24349,13 @@
     </row>
     <row r="207" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B207" s="167" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="C207" s="207" t="s">
+        <v>1610</v>
+      </c>
+      <c r="D207" s="207" t="s">
         <v>1611</v>
-      </c>
-      <c r="D207" s="207" t="s">
-        <v>1612</v>
       </c>
       <c r="E207" s="129" t="s">
         <v>1419</v>
@@ -24351,7 +24363,7 @@
       <c r="F207" s="166"/>
       <c r="G207" s="207"/>
       <c r="H207" s="208" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="I207" s="208"/>
       <c r="J207" s="208"/>
@@ -24372,13 +24384,13 @@
     </row>
     <row r="208" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B208" s="167" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C208" s="207" t="s">
         <v>1630</v>
       </c>
-      <c r="C208" s="207" t="s">
+      <c r="D208" s="207" t="s">
         <v>1631</v>
-      </c>
-      <c r="D208" s="207" t="s">
-        <v>1632</v>
       </c>
       <c r="E208" s="166" t="s">
         <v>1424</v>
@@ -24407,13 +24419,13 @@
     </row>
     <row r="209" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B209" s="167" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="C209" s="207" t="s">
+        <v>1632</v>
+      </c>
+      <c r="D209" s="207" t="s">
         <v>1633</v>
-      </c>
-      <c r="D209" s="207" t="s">
-        <v>1634</v>
       </c>
       <c r="E209" s="166" t="s">
         <v>1424</v>
@@ -24442,7 +24454,7 @@
     </row>
     <row r="210" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B210" s="167" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
   </sheetData>
@@ -25581,9 +25593,9 @@
       <c r="A20" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="B20" s="141" t="str">
+      <c r="B20" s="141">
         <f>Data!H90</f>
-        <v>LIBOR 2 month</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -25667,9 +25679,9 @@
       <c r="A36" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="B36" s="112" t="str">
+      <c r="B36" s="112">
         <f>Data!H98</f>
-        <v>Secured Assets</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -25692,7 +25704,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B42" s="44" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -25731,7 +25743,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LP WIP - IGFLend
</commit_message>
<xml_diff>
--- a/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.3.xlsx
+++ b/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ShrForms\specifications\lp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4258D0E9-214C-4C89-AD54-74A07A867A3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB6837C-62AD-4595-8AEA-E6016CFBD571}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="804" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2694" uniqueCount="1639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="1638">
   <si>
     <t>Field ID</t>
   </si>
@@ -4266,9 +4266,6 @@
   </si>
   <si>
     <t>Checkbox</t>
-  </si>
-  <si>
-    <t>4. Amount Provided must be greater than 0</t>
   </si>
   <si>
     <t>5. Balance Outstanding as at date of return cannot be greater than Amount Provided</t>
@@ -5918,7 +5915,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -6480,6 +6477,9 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -8391,7 +8391,7 @@
         <v>1010</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
   </sheetData>
@@ -8461,7 +8461,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="B10" s="140" t="e">
         <f>Data!#REF!</f>
@@ -8479,7 +8479,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="44" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="B14" s="150" t="str">
         <f>Data!I139</f>
@@ -8497,7 +8497,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="B18" s="141" t="str">
         <f>Data!H141</f>
@@ -8555,7 +8555,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="44" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="B30">
         <f>Data!H147</f>
@@ -8567,7 +8567,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="44" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="B32">
         <f>Data!H148</f>
@@ -8621,12 +8621,12 @@
     </row>
     <row r="43" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43" s="146" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="44" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="B44" s="112">
         <f>Data!H154</f>
@@ -8653,12 +8653,12 @@
     </row>
     <row r="50" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="146" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="44" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="B52" t="b">
         <f>Data!H157</f>
@@ -8685,7 +8685,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="44" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="B58" s="113" t="str">
         <f>Data!H160</f>
@@ -8703,7 +8703,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="44" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="B62" s="141">
         <f>Data!H162</f>
@@ -8715,7 +8715,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="44" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="B64" s="112" t="str">
         <f>Data!H163</f>
@@ -8724,7 +8724,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="44" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="B66" s="112">
         <f>Data!H164</f>
@@ -8742,7 +8742,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B70" s="44" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -8783,7 +8783,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -8829,7 +8829,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
   </sheetData>
@@ -8866,7 +8866,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="B3" s="140" t="e">
         <f>Data!I168</f>
@@ -8875,7 +8875,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="44" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="B5" s="140" t="str">
         <f>Data!I169</f>
@@ -8884,7 +8884,7 @@
     </row>
     <row r="7" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="44" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B7" s="140">
         <f>Data!I170</f>
@@ -8970,7 +8970,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="B3" s="140" t="e">
         <f>Data!#REF!</f>
@@ -8979,7 +8979,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="44" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="B5" s="140" t="e">
         <f>Data!#REF!</f>
@@ -8988,7 +8988,7 @@
     </row>
     <row r="7" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="44" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B7" s="140">
         <f>Data!I178</f>
@@ -8997,7 +8997,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="44" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="B9" t="str">
         <f>Data!H179</f>
@@ -9018,7 +9018,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="44" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="B13" s="112">
         <f>Data!H181</f>
@@ -9027,7 +9027,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="44" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="B15" s="112">
         <f>Data!H182</f>
@@ -9036,7 +9036,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="44" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="B17">
         <f>Data!H183</f>
@@ -9045,7 +9045,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="44" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="B19">
         <f>Data!H184</f>
@@ -9054,7 +9054,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="44" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="B21" t="b">
         <f>Data!H185</f>
@@ -14192,7 +14192,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -14200,7 +14200,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="33" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -14233,16 +14233,16 @@
         <v>349</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>350</v>
       </c>
       <c r="D1" s="31" t="s">
+        <v>1557</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>1558</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>1559</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>148</v>
@@ -14495,18 +14495,18 @@
     </row>
     <row r="2" spans="1:251" x14ac:dyDescent="0.2">
       <c r="A2" s="89" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="B2" s="89"/>
       <c r="C2" s="89" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="D2" s="89"/>
       <c r="E2" s="89" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="3" spans="1:251" x14ac:dyDescent="0.2">
@@ -14527,18 +14527,18 @@
     </row>
     <row r="4" spans="1:251" x14ac:dyDescent="0.2">
       <c r="A4" s="89" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="B4" s="89"/>
       <c r="C4" s="89" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="D4" s="89"/>
       <c r="E4" s="89" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="5" spans="1:251" x14ac:dyDescent="0.2">
@@ -14547,14 +14547,14 @@
       </c>
       <c r="B5" s="39"/>
       <c r="C5" s="33" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="33" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="6" spans="1:251" x14ac:dyDescent="0.2">
@@ -14563,14 +14563,14 @@
       </c>
       <c r="B6" s="39"/>
       <c r="C6" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="D6" s="33"/>
       <c r="E6" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="7" spans="1:251" x14ac:dyDescent="0.2">
@@ -14595,11 +14595,11 @@
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="33" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="D8" s="33"/>
       <c r="E8" s="33" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="F8" s="34" t="s">
         <v>1011</v>
@@ -14643,11 +14643,11 @@
       </c>
       <c r="B11" s="39"/>
       <c r="C11" s="89" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="89" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="F11" s="89" t="s">
         <v>1014</v>
@@ -14659,10 +14659,10 @@
       </c>
       <c r="B12" s="39"/>
       <c r="C12" s="33" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="F12" s="39" t="s">
         <v>1021</v>
@@ -15255,7 +15255,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -15272,8 +15272,8 @@
   <dimension ref="A1:AA210"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E101" sqref="E101"/>
+      <pane ySplit="8" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15310,14 +15310,14 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B2" s="157" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="C2" s="158"/>
       <c r="D2" s="156"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B3" s="159" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="C3" s="159"/>
       <c r="D3" s="160"/>
@@ -15327,12 +15327,12 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B4" s="159" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="C4" s="159"/>
       <c r="D4" s="161"/>
       <c r="G4" s="205" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -15356,10 +15356,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>1326</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>1327</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>1</v>
@@ -15398,28 +15398,28 @@
         <v>1261</v>
       </c>
       <c r="Q8" s="11" t="s">
+        <v>1327</v>
+      </c>
+      <c r="R8" s="11" t="s">
         <v>1328</v>
       </c>
-      <c r="R8" s="11" t="s">
-        <v>1329</v>
-      </c>
       <c r="S8" s="11" t="s">
+        <v>1537</v>
+      </c>
+      <c r="T8" s="11" t="s">
         <v>1538</v>
       </c>
-      <c r="T8" s="11" t="s">
+      <c r="U8" s="11" t="s">
         <v>1539</v>
       </c>
-      <c r="U8" s="11" t="s">
-        <v>1540</v>
-      </c>
       <c r="V8" s="11" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="W8" s="11" t="s">
+        <v>1553</v>
+      </c>
+      <c r="X8" s="11" t="s">
         <v>1554</v>
-      </c>
-      <c r="X8" s="11" t="s">
-        <v>1555</v>
       </c>
       <c r="Y8" s="11" t="s">
         <v>140</v>
@@ -15514,7 +15514,7 @@
         <v>Submission.LPR003</v>
       </c>
       <c r="D11" s="109" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="E11" s="108" t="s">
         <v>132</v>
@@ -15528,7 +15528,7 @@
       </c>
       <c r="I11" s="107"/>
       <c r="J11" s="101" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="K11" s="108" t="s">
         <v>133</v>
@@ -15556,14 +15556,14 @@
     <row r="12" spans="1:27" ht="114.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="23" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="C12" s="23" t="str">
         <f t="shared" si="0"/>
         <v>Submission.LPR003a</v>
       </c>
       <c r="D12" s="88" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>1268</v>
@@ -15583,7 +15583,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="168"/>
       <c r="N12" s="10" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="O12" s="102"/>
       <c r="P12" s="10"/>
@@ -15612,7 +15612,7 @@
         <v>Submission.LPR005</v>
       </c>
       <c r="D13" s="109" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="E13" s="108" t="s">
         <v>130</v>
@@ -15650,14 +15650,14 @@
     <row r="14" spans="1:27" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="23" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="C14" s="23" t="str">
         <f t="shared" si="0"/>
         <v>Submission.LPR005a</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>130</v>
@@ -15722,7 +15722,7 @@
       <c r="L15" s="10"/>
       <c r="M15" s="102"/>
       <c r="N15" s="16" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="O15" s="102"/>
       <c r="P15" s="10"/>
@@ -15891,7 +15891,7 @@
       </c>
       <c r="F19" s="108"/>
       <c r="G19" s="109" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="H19" s="103"/>
       <c r="I19" s="107">
@@ -16018,7 +16018,7 @@
     <row r="22" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
       <c r="B22" s="179" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="C22" s="179" t="str">
         <f>"Submission." &amp; B22</f>
@@ -16028,7 +16028,7 @@
         <v>1012</v>
       </c>
       <c r="E22" s="181" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="F22" s="183"/>
       <c r="G22" s="183"/>
@@ -16055,7 +16055,7 @@
     <row r="23" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
       <c r="B23" s="179" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="C23" s="179" t="str">
         <f t="shared" ref="C23" si="1">"Submission." &amp; B23</f>
@@ -16065,7 +16065,7 @@
         <v>896</v>
       </c>
       <c r="E23" s="181" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="F23" s="183"/>
       <c r="G23" s="183"/>
@@ -16092,17 +16092,17 @@
     <row r="24" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
       <c r="B24" s="179" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="C24" s="179" t="str">
         <f t="shared" si="0"/>
         <v>Submission.LPR100</v>
       </c>
       <c r="D24" s="180" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="E24" s="182" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="F24" s="183"/>
       <c r="G24" s="183"/>
@@ -16129,17 +16129,17 @@
     <row r="25" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
       <c r="B25" s="179" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="C25" s="179" t="str">
         <f t="shared" ref="C25" si="2">"Submission." &amp; B25</f>
         <v>Submission.LPR101</v>
       </c>
       <c r="D25" s="180" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="E25" s="181" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="F25" s="183"/>
       <c r="G25" s="183"/>
@@ -16294,14 +16294,15 @@
         <v>IGFLend.LPIGF001</v>
       </c>
       <c r="D29" s="109" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="E29" s="108" t="s">
         <v>1271</v>
       </c>
       <c r="F29" s="108"/>
-      <c r="G29" s="109" t="s">
-        <v>1337</v>
+      <c r="G29" s="109" t="str">
+        <f>Pfo_Page_Serial_Padded_4</f>
+        <v>0002</v>
       </c>
       <c r="H29" s="103"/>
       <c r="I29" s="169">
@@ -16451,13 +16452,8 @@
       <c r="L32" s="10" t="s">
         <v>1265</v>
       </c>
-      <c r="M32" s="102" t="b">
-        <f>H32&gt;0</f>
-        <v>1</v>
-      </c>
-      <c r="N32" s="10" t="s">
-        <v>1306</v>
-      </c>
+      <c r="M32" s="102"/>
+      <c r="N32" s="10"/>
       <c r="O32" s="102"/>
       <c r="P32" s="10"/>
       <c r="Q32" s="102"/>
@@ -16505,7 +16501,7 @@
         <v>1</v>
       </c>
       <c r="N33" s="10" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="O33" s="102"/>
       <c r="P33" s="10"/>
@@ -16538,8 +16534,8 @@
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
-      <c r="H34" s="104" t="s">
-        <v>929</v>
+      <c r="H34" s="104">
+        <v>4</v>
       </c>
       <c r="I34" s="105"/>
       <c r="J34" s="101"/>
@@ -16589,7 +16585,7 @@
       </c>
       <c r="I35" s="105"/>
       <c r="J35" s="115" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>131</v>
@@ -16597,7 +16593,7 @@
       <c r="L35" s="10"/>
       <c r="M35" s="102"/>
       <c r="N35" s="16" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="O35" s="102"/>
       <c r="P35" s="10"/>
@@ -16607,7 +16603,10 @@
       <c r="T35" s="10"/>
       <c r="U35" s="102"/>
       <c r="V35" s="10"/>
-      <c r="W35" s="10"/>
+      <c r="W35" s="10" t="b">
+        <f>H34&lt;&gt;4</f>
+        <v>0</v>
+      </c>
       <c r="X35" s="10"/>
       <c r="Y35" s="16" t="s">
         <v>215</v>
@@ -16643,12 +16642,9 @@
       <c r="L36" s="10" t="s">
         <v>1265</v>
       </c>
-      <c r="M36" s="102" t="b">
-        <f>H36&gt;0</f>
-        <v>1</v>
-      </c>
+      <c r="M36" s="102"/>
       <c r="N36" s="10" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="O36" s="102"/>
       <c r="P36" s="10"/>
@@ -16676,7 +16672,7 @@
         <v>IGFLend.LPIGF009</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>130</v>
@@ -16722,7 +16718,7 @@
         <v>IGFLend.LPIGF010</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>130</v>
@@ -16745,7 +16741,7 @@
         <v>1</v>
       </c>
       <c r="N38" s="10" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="O38" s="102"/>
       <c r="P38" s="10"/>
@@ -16824,8 +16820,8 @@
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
-      <c r="H40" s="103" t="s">
-        <v>930</v>
+      <c r="H40" s="103">
+        <v>3</v>
       </c>
       <c r="I40" s="105"/>
       <c r="J40" s="101"/>
@@ -16875,7 +16871,7 @@
       </c>
       <c r="I41" s="105"/>
       <c r="J41" s="115" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="K41" s="9" t="s">
         <v>131</v>
@@ -16883,7 +16879,7 @@
       <c r="L41" s="10"/>
       <c r="M41" s="102"/>
       <c r="N41" s="16" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="O41" s="102"/>
       <c r="P41" s="10"/>
@@ -16893,7 +16889,10 @@
       <c r="T41" s="10"/>
       <c r="U41" s="102"/>
       <c r="V41" s="10"/>
-      <c r="W41" s="10"/>
+      <c r="W41" s="10" t="b">
+        <f>H40=3</f>
+        <v>1</v>
+      </c>
       <c r="X41" s="10"/>
       <c r="Y41" s="16" t="s">
         <v>221</v>
@@ -16923,7 +16922,7 @@
       </c>
       <c r="I42" s="105"/>
       <c r="J42" s="115" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="K42" s="9" t="s">
         <v>131</v>
@@ -16931,7 +16930,7 @@
       <c r="L42" s="10"/>
       <c r="M42" s="102"/>
       <c r="N42" s="16" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="O42" s="102"/>
       <c r="P42" s="10"/>
@@ -16941,7 +16940,10 @@
       <c r="T42" s="10"/>
       <c r="U42" s="102"/>
       <c r="V42" s="10"/>
-      <c r="W42" s="10"/>
+      <c r="W42" s="10" t="b">
+        <f>H40=3</f>
+        <v>1</v>
+      </c>
       <c r="X42" s="10"/>
       <c r="Y42" s="16" t="s">
         <v>222</v>
@@ -16977,22 +16979,20 @@
       <c r="L43" s="10"/>
       <c r="M43" s="102"/>
       <c r="N43" s="10" t="s">
-        <v>1324</v>
-      </c>
-      <c r="O43" s="102" t="b">
-        <f>H43&gt;0</f>
-        <v>1</v>
-      </c>
-      <c r="P43" s="10" t="s">
-        <v>1316</v>
-      </c>
+        <v>1323</v>
+      </c>
+      <c r="O43" s="102"/>
+      <c r="P43" s="10"/>
       <c r="Q43" s="102"/>
       <c r="R43" s="10"/>
       <c r="S43" s="102"/>
       <c r="T43" s="10"/>
       <c r="U43" s="102"/>
       <c r="V43" s="10"/>
-      <c r="W43" s="10"/>
+      <c r="W43" s="10" t="b">
+        <f>H40=3</f>
+        <v>1</v>
+      </c>
       <c r="X43" s="10"/>
       <c r="Y43" s="16" t="s">
         <v>223</v>
@@ -17015,8 +17015,8 @@
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="17"/>
-      <c r="H44" s="103" t="s">
-        <v>930</v>
+      <c r="H44" s="103">
+        <v>3</v>
       </c>
       <c r="I44" s="105"/>
       <c r="J44" s="101"/>
@@ -17057,7 +17057,7 @@
         <v>1285</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
@@ -17072,7 +17072,7 @@
       <c r="L45" s="10"/>
       <c r="M45" s="102"/>
       <c r="N45" s="16" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="O45" s="102"/>
       <c r="P45" s="16"/>
@@ -17082,7 +17082,10 @@
       <c r="T45" s="16"/>
       <c r="U45" s="102"/>
       <c r="V45" s="16"/>
-      <c r="W45" s="16"/>
+      <c r="W45" s="16" t="b">
+        <f>H44=3</f>
+        <v>1</v>
+      </c>
       <c r="X45" s="16"/>
       <c r="Y45" s="16" t="s">
         <v>370</v>
@@ -17118,22 +17121,20 @@
       <c r="L46" s="10"/>
       <c r="M46" s="102"/>
       <c r="N46" s="16" t="s">
-        <v>1320</v>
-      </c>
-      <c r="O46" s="102" t="b">
-        <f>H46&gt;0</f>
-        <v>1</v>
-      </c>
-      <c r="P46" s="10" t="s">
-        <v>1321</v>
-      </c>
+        <v>1319</v>
+      </c>
+      <c r="O46" s="102"/>
+      <c r="P46" s="10"/>
       <c r="Q46" s="102"/>
       <c r="R46" s="10"/>
       <c r="S46" s="102"/>
       <c r="T46" s="10"/>
       <c r="U46" s="102"/>
       <c r="V46" s="10"/>
-      <c r="W46" s="10"/>
+      <c r="W46" s="10" t="b">
+        <f>H44=3</f>
+        <v>1</v>
+      </c>
       <c r="X46" s="10"/>
       <c r="Y46" s="16" t="s">
         <v>225</v>
@@ -17169,7 +17170,7 @@
       <c r="L47" s="10"/>
       <c r="M47" s="102"/>
       <c r="N47" s="16" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="O47" s="102"/>
       <c r="P47" s="10"/>
@@ -17179,7 +17180,10 @@
       <c r="T47" s="10"/>
       <c r="U47" s="102"/>
       <c r="V47" s="10"/>
-      <c r="W47" s="10"/>
+      <c r="W47" s="212" t="b">
+        <f>H44=3</f>
+        <v>1</v>
+      </c>
       <c r="X47" s="10"/>
       <c r="Y47" s="16" t="s">
         <v>226</v>
@@ -17215,7 +17219,7 @@
       <c r="L48" s="10"/>
       <c r="M48" s="102"/>
       <c r="N48" s="16" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="O48" s="102"/>
       <c r="P48" s="16"/>
@@ -17225,7 +17229,10 @@
       <c r="T48" s="16"/>
       <c r="U48" s="102"/>
       <c r="V48" s="16"/>
-      <c r="W48" s="16"/>
+      <c r="W48" s="180" t="b">
+        <f>H44=3</f>
+        <v>1</v>
+      </c>
       <c r="X48" s="16"/>
       <c r="Y48" s="16" t="s">
         <v>227</v>
@@ -17236,7 +17243,7 @@
     </row>
     <row r="49" spans="1:26" ht="95.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="23" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="C49" s="119" t="str">
         <f t="shared" si="3"/>
@@ -17261,7 +17268,7 @@
       <c r="L49" s="10"/>
       <c r="M49" s="102"/>
       <c r="N49" s="16" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="O49" s="102"/>
       <c r="P49" s="16"/>
@@ -17271,7 +17278,10 @@
       <c r="T49" s="16"/>
       <c r="U49" s="102"/>
       <c r="V49" s="16"/>
-      <c r="W49" s="16"/>
+      <c r="W49" s="180" t="b">
+        <f>H44=3</f>
+        <v>1</v>
+      </c>
       <c r="X49" s="16"/>
       <c r="Y49" s="16" t="s">
         <v>228</v>
@@ -17280,14 +17290,14 @@
     </row>
     <row r="50" spans="1:26" ht="71.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="23" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="C50" s="119" t="str">
         <f t="shared" si="3"/>
         <v>IGFLend.LPIGF020b</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>1304</v>
@@ -17305,7 +17315,7 @@
       <c r="L50" s="10"/>
       <c r="M50" s="102"/>
       <c r="N50" s="10" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="O50" s="102"/>
       <c r="P50" s="10"/>
@@ -17315,7 +17325,10 @@
       <c r="T50" s="10"/>
       <c r="U50" s="102"/>
       <c r="V50" s="10"/>
-      <c r="W50" s="10"/>
+      <c r="W50" s="212" t="b">
+        <f>H44=3</f>
+        <v>1</v>
+      </c>
       <c r="X50" s="10"/>
       <c r="Y50" s="16" t="s">
         <v>228</v>
@@ -17349,7 +17362,7 @@
       <c r="L51" s="10"/>
       <c r="M51" s="102"/>
       <c r="N51" s="10" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="O51" s="102"/>
       <c r="P51" s="16"/>
@@ -17384,8 +17397,8 @@
       </c>
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
-      <c r="H52" s="103" t="s">
-        <v>930</v>
+      <c r="H52" s="103">
+        <v>3</v>
       </c>
       <c r="I52" s="105"/>
       <c r="J52" s="101"/>
@@ -17423,7 +17436,7 @@
         <v>IGFLend.LPIGF022</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>134</v>
@@ -17441,7 +17454,7 @@
       <c r="L53" s="10"/>
       <c r="M53" s="102"/>
       <c r="N53" s="16" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="O53" s="102"/>
       <c r="P53" s="10"/>
@@ -17451,7 +17464,10 @@
       <c r="T53" s="10"/>
       <c r="U53" s="102"/>
       <c r="V53" s="10"/>
-      <c r="W53" s="10"/>
+      <c r="W53" s="10" t="b">
+        <f>H52=3</f>
+        <v>1</v>
+      </c>
       <c r="X53" s="10"/>
       <c r="Y53" s="16" t="s">
         <v>230</v>
@@ -17469,10 +17485,10 @@
         <v>IGFLend.LPIGF023</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="F54" s="17"/>
       <c r="G54" s="17"/>
@@ -17487,7 +17503,7 @@
       <c r="L54" s="10"/>
       <c r="M54" s="102"/>
       <c r="N54" s="16" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="O54" s="102"/>
       <c r="P54" s="10"/>
@@ -17497,7 +17513,10 @@
       <c r="T54" s="10"/>
       <c r="U54" s="102"/>
       <c r="V54" s="10"/>
-      <c r="W54" s="10"/>
+      <c r="W54" s="10" t="b">
+        <f>H52=3</f>
+        <v>1</v>
+      </c>
       <c r="X54" s="10"/>
       <c r="Y54" s="16" t="s">
         <v>231</v>
@@ -17527,7 +17546,7 @@
       </c>
       <c r="I55" s="105"/>
       <c r="J55" s="104" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="K55" s="23" t="s">
         <v>133</v>
@@ -17583,7 +17602,7 @@
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B57" s="119" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="C57" s="119" t="str">
         <f>"IGFBorrow." &amp; B57</f>
@@ -17621,7 +17640,7 @@
       <c r="W57" s="16"/>
       <c r="X57" s="16"/>
       <c r="Y57" s="57" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="Z57" s="10" t="s">
         <v>409</v>
@@ -17644,7 +17663,7 @@
       <c r="F58" s="17"/>
       <c r="G58" s="17"/>
       <c r="H58" s="104" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="I58" s="105"/>
       <c r="J58" s="101"/>
@@ -17676,14 +17695,14 @@
     <row r="59" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="15"/>
       <c r="B59" s="108" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="C59" s="119" t="str">
         <f t="shared" si="4"/>
         <v>IGFBorrow.LPIGF100</v>
       </c>
       <c r="D59" s="109" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="E59" s="108" t="s">
         <v>1271</v>
@@ -17692,7 +17711,7 @@
         <v>1262</v>
       </c>
       <c r="G59" s="109" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="H59" s="103"/>
       <c r="I59" s="107">
@@ -17740,7 +17759,7 @@
       <c r="F60" s="17"/>
       <c r="G60" s="17"/>
       <c r="H60" s="104" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="I60" s="105"/>
       <c r="J60" s="101"/>
@@ -17845,7 +17864,7 @@
         <v>1</v>
       </c>
       <c r="N62" s="10" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="O62" s="102"/>
       <c r="P62" s="10"/>
@@ -17894,7 +17913,7 @@
         <v>1</v>
       </c>
       <c r="N63" s="10" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="O63" s="102"/>
       <c r="P63" s="10"/>
@@ -17978,7 +17997,7 @@
       </c>
       <c r="I65" s="105"/>
       <c r="J65" s="115" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="K65" s="9" t="s">
         <v>131</v>
@@ -17986,7 +18005,7 @@
       <c r="L65" s="10"/>
       <c r="M65" s="102"/>
       <c r="N65" s="16" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="O65" s="102"/>
       <c r="P65" s="10"/>
@@ -18037,7 +18056,7 @@
         <v>1</v>
       </c>
       <c r="N66" s="10" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="O66" s="102"/>
       <c r="P66" s="10"/>
@@ -18065,7 +18084,7 @@
         <v>IGFBorrow.LPIGF033</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>130</v>
@@ -18111,7 +18130,7 @@
         <v>IGFBorrow.LPIGF034</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="E68" s="9" t="s">
         <v>130</v>
@@ -18134,7 +18153,7 @@
         <v>1</v>
       </c>
       <c r="N68" s="10" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="O68" s="102"/>
       <c r="P68" s="10"/>
@@ -18264,7 +18283,7 @@
       </c>
       <c r="I71" s="105"/>
       <c r="J71" s="115" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="K71" s="9" t="s">
         <v>131</v>
@@ -18272,7 +18291,7 @@
       <c r="L71" s="10"/>
       <c r="M71" s="102"/>
       <c r="N71" s="16" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="O71" s="102"/>
       <c r="P71" s="10"/>
@@ -18312,7 +18331,7 @@
       </c>
       <c r="I72" s="105"/>
       <c r="J72" s="115" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="K72" s="9" t="s">
         <v>131</v>
@@ -18320,7 +18339,7 @@
       <c r="L72" s="10"/>
       <c r="M72" s="102"/>
       <c r="N72" s="16" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="O72" s="102"/>
       <c r="P72" s="10"/>
@@ -18366,14 +18385,14 @@
       <c r="L73" s="10"/>
       <c r="M73" s="102"/>
       <c r="N73" s="10" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="O73" s="102" t="b">
         <f>H73&gt;0</f>
         <v>1</v>
       </c>
       <c r="P73" s="10" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="Q73" s="102"/>
       <c r="R73" s="10"/>
@@ -18446,7 +18465,7 @@
         <v>1285</v>
       </c>
       <c r="E75" s="23" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="F75" s="17"/>
       <c r="G75" s="17"/>
@@ -18461,7 +18480,7 @@
       <c r="L75" s="10"/>
       <c r="M75" s="102"/>
       <c r="N75" s="16" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="O75" s="102"/>
       <c r="P75" s="16"/>
@@ -18489,7 +18508,7 @@
         <v>IGFBorrow.LPIGF041</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="E76" s="111" t="s">
         <v>1271</v>
@@ -18507,14 +18526,14 @@
       <c r="L76" s="10"/>
       <c r="M76" s="102"/>
       <c r="N76" s="16" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="O76" s="102" t="b">
         <f>H76&gt;0</f>
         <v>1</v>
       </c>
       <c r="P76" s="10" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="Q76" s="102"/>
       <c r="R76" s="10"/>
@@ -18558,7 +18577,7 @@
       <c r="L77" s="10"/>
       <c r="M77" s="102"/>
       <c r="N77" s="16" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="O77" s="102"/>
       <c r="P77" s="10"/>
@@ -18604,7 +18623,7 @@
       <c r="L78" s="10"/>
       <c r="M78" s="102"/>
       <c r="N78" s="16" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="O78" s="102"/>
       <c r="P78" s="16"/>
@@ -18625,7 +18644,7 @@
     </row>
     <row r="79" spans="2:26" ht="81.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="23" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="C79" s="119" t="str">
         <f t="shared" si="4"/>
@@ -18650,7 +18669,7 @@
       <c r="L79" s="10"/>
       <c r="M79" s="102"/>
       <c r="N79" s="16" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="O79" s="102"/>
       <c r="P79" s="16"/>
@@ -18676,7 +18695,7 @@
         <v>IGFBorrow.LPIGF044b</v>
       </c>
       <c r="D80" s="16" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="E80" s="9" t="s">
         <v>1304</v>
@@ -18694,7 +18713,7 @@
       <c r="L80" s="10"/>
       <c r="M80" s="102"/>
       <c r="N80" s="10" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="O80" s="102"/>
       <c r="P80" s="10"/>
@@ -18713,7 +18732,7 @@
     </row>
     <row r="81" spans="1:26" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="23" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="C81" s="119" t="str">
         <f t="shared" si="4"/>
@@ -18738,7 +18757,7 @@
       <c r="L81" s="10"/>
       <c r="M81" s="102"/>
       <c r="N81" s="10" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="O81" s="102"/>
       <c r="P81" s="16"/>
@@ -18766,7 +18785,7 @@
         <v>IGFBorrow.LPIGF045</v>
       </c>
       <c r="D82" s="16" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="E82" s="7" t="s">
         <v>1305</v>
@@ -18778,7 +18797,7 @@
       </c>
       <c r="I82" s="105"/>
       <c r="J82" s="104" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="K82" s="23" t="s">
         <v>133</v>
@@ -18859,7 +18878,7 @@
       <c r="L84" s="10"/>
       <c r="M84" s="102"/>
       <c r="N84" s="10" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="O84" s="102"/>
       <c r="P84" s="10"/>
@@ -18888,7 +18907,7 @@
         <v>ISDA.LPC019</v>
       </c>
       <c r="D85" s="109" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="E85" s="108" t="s">
         <v>1271</v>
@@ -18897,7 +18916,7 @@
         <v>1262</v>
       </c>
       <c r="G85" s="109" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="H85" s="103"/>
       <c r="I85" s="107">
@@ -18938,7 +18957,7 @@
         <v>175</v>
       </c>
       <c r="E86" s="23" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="F86" s="17"/>
       <c r="G86" s="17"/>
@@ -19094,7 +19113,7 @@
         <v>1</v>
       </c>
       <c r="N89" s="10" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="O89" s="102"/>
       <c r="P89" s="10"/>
@@ -19168,7 +19187,7 @@
         <v>ISDA.LPC025</v>
       </c>
       <c r="D91" s="16" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="E91" s="9" t="s">
         <v>1304</v>
@@ -19186,7 +19205,7 @@
       <c r="L91" s="10"/>
       <c r="M91" s="102"/>
       <c r="N91" s="16" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="O91" s="102"/>
       <c r="P91" s="16"/>
@@ -19208,14 +19227,14 @@
     </row>
     <row r="92" spans="1:26" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="23" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="C92" s="119" t="str">
         <f t="shared" si="5"/>
         <v>ISDA.LPC025a</v>
       </c>
       <c r="D92" s="16" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="E92" s="9" t="s">
         <v>1304</v>
@@ -19233,7 +19252,7 @@
       <c r="L92" s="10"/>
       <c r="M92" s="102"/>
       <c r="N92" s="10" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="O92" s="102"/>
       <c r="P92" s="10"/>
@@ -19280,7 +19299,7 @@
       <c r="L93" s="10"/>
       <c r="M93" s="102"/>
       <c r="N93" s="10" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="O93" s="102"/>
       <c r="P93" s="16"/>
@@ -19311,7 +19330,7 @@
         <v>179</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="F94" s="17"/>
       <c r="G94" s="17"/>
@@ -19355,7 +19374,7 @@
         <v>180</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="F95" s="17"/>
       <c r="G95" s="17"/>
@@ -19421,7 +19440,7 @@
         <v>0</v>
       </c>
       <c r="N96" s="10" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="O96" s="102"/>
       <c r="P96" s="10"/>
@@ -19450,7 +19469,7 @@
         <v>182</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="F97" s="17"/>
       <c r="G97" s="17"/>
@@ -19496,7 +19515,7 @@
         <v>183</v>
       </c>
       <c r="E98" s="23" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="F98" s="17"/>
       <c r="G98" s="17"/>
@@ -19542,7 +19561,7 @@
         <v>184</v>
       </c>
       <c r="E99" s="23" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="F99" s="17"/>
       <c r="G99" s="17"/>
@@ -19557,7 +19576,7 @@
       <c r="L99" s="10"/>
       <c r="M99" s="102"/>
       <c r="N99" s="10" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="O99" s="102"/>
       <c r="P99" s="10"/>
@@ -19589,7 +19608,7 @@
         <v>185</v>
       </c>
       <c r="E100" s="23" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="F100" s="17"/>
       <c r="G100" s="17"/>
@@ -19626,7 +19645,7 @@
     <row r="101" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="15"/>
       <c r="B101" s="179" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="C101" s="186" t="str">
         <f>"ISDA." &amp; B101</f>
@@ -19636,7 +19655,7 @@
         <v>1011</v>
       </c>
       <c r="E101" s="182" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="F101" s="183"/>
       <c r="G101" s="183"/>
@@ -19699,7 +19718,7 @@
       </c>
       <c r="C103" s="172"/>
       <c r="D103" s="173" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="E103" s="172" t="s">
         <v>1271</v>
@@ -19708,7 +19727,7 @@
         <v>1262</v>
       </c>
       <c r="G103" s="173" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="H103" s="174"/>
       <c r="I103" s="175"/>
@@ -19744,7 +19763,7 @@
         <v>ISDACovenant.LPC003a</v>
       </c>
       <c r="D104" s="109" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="E104" s="108" t="s">
         <v>1271</v>
@@ -19796,7 +19815,7 @@
         <v>340</v>
       </c>
       <c r="E105" s="23" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="F105" s="17"/>
       <c r="G105" s="17"/>
@@ -19848,7 +19867,7 @@
       <c r="F106" s="17"/>
       <c r="G106" s="17"/>
       <c r="H106" s="104" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="I106" s="105"/>
       <c r="J106" s="101"/>
@@ -19858,7 +19877,7 @@
       <c r="L106" s="10"/>
       <c r="M106" s="102"/>
       <c r="N106" s="10" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="O106" s="102"/>
       <c r="P106" s="10"/>
@@ -19895,7 +19914,7 @@
       <c r="F107" s="17"/>
       <c r="G107" s="17"/>
       <c r="H107" s="149" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="I107" s="105"/>
       <c r="J107" s="101"/>
@@ -19937,7 +19956,7 @@
         <v>342</v>
       </c>
       <c r="E108" s="23" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="F108" s="17"/>
       <c r="G108" s="17"/>
@@ -20036,7 +20055,7 @@
       <c r="F110" s="17"/>
       <c r="G110" s="17"/>
       <c r="H110" s="149" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="I110" s="105"/>
       <c r="J110" s="101"/>
@@ -20119,7 +20138,7 @@
       <c r="L112" s="10"/>
       <c r="M112" s="102"/>
       <c r="N112" s="10" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="O112" s="102"/>
       <c r="P112" s="10"/>
@@ -20147,10 +20166,10 @@
         <v>Facility.LPF001</v>
       </c>
       <c r="D113" s="16" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="E113" s="23" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="F113" s="17"/>
       <c r="G113" s="17"/>
@@ -20159,7 +20178,7 @@
       </c>
       <c r="I113" s="105"/>
       <c r="J113" s="104" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="K113" s="9" t="s">
         <v>131</v>
@@ -20244,7 +20263,7 @@
         <v>346</v>
       </c>
       <c r="E115" s="23" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="F115" s="17"/>
       <c r="G115" s="17"/>
@@ -20259,7 +20278,7 @@
       <c r="L115" s="10"/>
       <c r="M115" s="102"/>
       <c r="N115" s="43" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="O115" s="102"/>
       <c r="P115" s="10"/>
@@ -20291,14 +20310,14 @@
         <v>Facility.LPF004</v>
       </c>
       <c r="D116" s="109" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="E116" s="108" t="s">
         <v>137</v>
       </c>
       <c r="F116" s="108"/>
       <c r="G116" s="109" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="H116" s="103"/>
       <c r="I116" s="120" t="str">
@@ -20306,7 +20325,7 @@
         <v>DMOBOS0002</v>
       </c>
       <c r="J116" s="120" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="K116" s="108"/>
       <c r="L116" s="109"/>
@@ -20384,10 +20403,10 @@
         <v>Facility.LPF005b</v>
       </c>
       <c r="D118" s="16" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="E118" s="23" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="F118" s="17"/>
       <c r="G118" s="17"/>
@@ -20402,7 +20421,7 @@
       <c r="L118" s="10"/>
       <c r="M118" s="102"/>
       <c r="N118" s="10" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="O118" s="102"/>
       <c r="P118" s="10"/>
@@ -20499,7 +20518,7 @@
         <v>1</v>
       </c>
       <c r="N120" s="10" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="O120" s="102"/>
       <c r="P120" s="10"/>
@@ -20550,14 +20569,14 @@
         <v>1</v>
       </c>
       <c r="N121" s="10" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="O121" s="123" t="b">
         <f>AND(ABS(H121-H14)&lt;=H202,ABS(H14-H121)&lt;=H202)</f>
         <v>1</v>
       </c>
       <c r="P121" s="10" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="Q121" s="102"/>
       <c r="R121" s="10"/>
@@ -20606,7 +20625,7 @@
         <v>1</v>
       </c>
       <c r="N122" s="10" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="O122" s="102"/>
       <c r="P122" s="10"/>
@@ -20655,11 +20674,11 @@
         <v>1</v>
       </c>
       <c r="N123" s="10" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="O123" s="102"/>
       <c r="P123" s="95" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="Q123" s="102"/>
       <c r="R123" s="10"/>
@@ -20706,7 +20725,7 @@
         <v>1</v>
       </c>
       <c r="N124" s="10" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="O124" s="102"/>
       <c r="P124" s="10"/>
@@ -20750,7 +20769,7 @@
       <c r="L125" s="10"/>
       <c r="M125" s="102"/>
       <c r="N125" s="10" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="O125" s="102"/>
       <c r="P125" s="10"/>
@@ -20781,7 +20800,7 @@
         <v>408</v>
       </c>
       <c r="E126" s="23" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="F126" s="17"/>
       <c r="G126" s="17"/>
@@ -20796,7 +20815,7 @@
       <c r="L126" s="10"/>
       <c r="M126" s="102"/>
       <c r="N126" s="10" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="O126" s="102"/>
       <c r="P126" s="10"/>
@@ -20824,7 +20843,7 @@
         <v>Facility.LPF014</v>
       </c>
       <c r="D127" s="16" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="E127" s="23" t="s">
         <v>138</v>
@@ -20832,7 +20851,7 @@
       <c r="F127" s="17"/>
       <c r="G127" s="17"/>
       <c r="H127" s="104" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="I127" s="105"/>
       <c r="J127" s="101"/>
@@ -20842,7 +20861,7 @@
       <c r="L127" s="10"/>
       <c r="M127" s="102"/>
       <c r="N127" s="10" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="O127" s="102"/>
       <c r="P127" s="10"/>
@@ -20891,7 +20910,7 @@
       <c r="L128" s="10"/>
       <c r="M128" s="102"/>
       <c r="N128" s="10" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="O128" s="102"/>
       <c r="P128" s="10"/>
@@ -20922,7 +20941,7 @@
         <v>536</v>
       </c>
       <c r="E129" s="23" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="F129" s="17"/>
       <c r="G129" s="17"/>
@@ -20966,7 +20985,7 @@
         <v>162</v>
       </c>
       <c r="E130" s="23" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="F130" s="17"/>
       <c r="G130" s="17"/>
@@ -21010,7 +21029,7 @@
         <v>163</v>
       </c>
       <c r="E131" s="23" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="F131" s="17"/>
       <c r="G131" s="17"/>
@@ -21051,7 +21070,7 @@
         <v>Facility.LPF019</v>
       </c>
       <c r="D132" s="16" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="E132" s="23" t="s">
         <v>138</v>
@@ -21059,7 +21078,7 @@
       <c r="F132" s="17"/>
       <c r="G132" s="17"/>
       <c r="H132" s="104" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="I132" s="105"/>
       <c r="J132" s="101"/>
@@ -21069,7 +21088,7 @@
       <c r="L132" s="10"/>
       <c r="M132" s="102"/>
       <c r="N132" s="10" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="O132" s="102"/>
       <c r="P132" s="10"/>
@@ -21098,10 +21117,10 @@
         <v>Facility.LPF020</v>
       </c>
       <c r="D133" s="16" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="E133" s="23" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="F133" s="17"/>
       <c r="G133" s="17"/>
@@ -21110,7 +21129,7 @@
       </c>
       <c r="I133" s="105"/>
       <c r="J133" s="101" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="K133" s="9" t="s">
         <v>133</v>
@@ -21138,7 +21157,7 @@
     <row r="134" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="15"/>
       <c r="B134" s="179" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="C134" s="186" t="str">
         <f>"Facility." &amp; B134</f>
@@ -21148,7 +21167,7 @@
         <v>1046</v>
       </c>
       <c r="E134" s="181" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="F134" s="183"/>
       <c r="G134" s="183"/>
@@ -21175,7 +21194,7 @@
     <row r="135" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="15"/>
       <c r="B135" s="179" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="C135" s="186" t="str">
         <f>"Facility." &amp; B135</f>
@@ -21185,7 +21204,7 @@
         <v>1014</v>
       </c>
       <c r="E135" s="181" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="F135" s="183"/>
       <c r="G135" s="183"/>
@@ -21265,7 +21284,7 @@
       <c r="L137" s="10"/>
       <c r="M137" s="102"/>
       <c r="N137" s="10" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="O137" s="102"/>
       <c r="P137" s="10"/>
@@ -21296,7 +21315,7 @@
         <v>164</v>
       </c>
       <c r="E138" s="23" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="F138" s="17"/>
       <c r="G138" s="17"/>
@@ -21313,7 +21332,7 @@
       </c>
       <c r="M138" s="117"/>
       <c r="N138" s="10" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="O138" s="102"/>
       <c r="P138" s="10"/>
@@ -21340,14 +21359,14 @@
         <v>Loan.LPL002b</v>
       </c>
       <c r="D139" s="109" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="E139" s="108" t="s">
         <v>137</v>
       </c>
       <c r="F139" s="108"/>
       <c r="G139" s="109" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="H139" s="104"/>
       <c r="I139" s="104" t="str">
@@ -21355,7 +21374,7 @@
         <v>BOSFIXED0002</v>
       </c>
       <c r="J139" s="120" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="K139" s="108"/>
       <c r="L139" s="109"/>
@@ -21391,7 +21410,7 @@
         <v>165</v>
       </c>
       <c r="E140" s="23" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="F140" s="17"/>
       <c r="G140" s="17"/>
@@ -21434,7 +21453,7 @@
         <v>Loan.LPL004</v>
       </c>
       <c r="D141" s="16" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="E141" s="23" t="s">
         <v>134</v>
@@ -21442,7 +21461,7 @@
       <c r="F141" s="17"/>
       <c r="G141" s="17"/>
       <c r="H141" s="104" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="I141" s="105"/>
       <c r="J141" s="101"/>
@@ -21452,7 +21471,7 @@
       <c r="L141" s="10"/>
       <c r="M141" s="102"/>
       <c r="N141" s="10" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="O141" s="102"/>
       <c r="P141" s="10"/>
@@ -21506,14 +21525,14 @@
         <v>1</v>
       </c>
       <c r="N142" s="10" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="O142" s="102" t="b">
         <f>H142&lt;=H121</f>
         <v>1</v>
       </c>
       <c r="P142" s="10" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="Q142" s="102"/>
       <c r="R142" s="10"/>
@@ -21562,14 +21581,14 @@
         <v>1</v>
       </c>
       <c r="N143" s="10" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="O143" s="102" t="b">
         <f>H143&lt;=H122</f>
         <v>1</v>
       </c>
       <c r="P143" s="10" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="Q143" s="102"/>
       <c r="R143" s="10"/>
@@ -21618,14 +21637,14 @@
         <v>1</v>
       </c>
       <c r="N144" s="10" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="O144" s="102" t="b">
         <f>H144&lt;=H123</f>
         <v>1</v>
       </c>
       <c r="P144" s="10" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="Q144" s="102"/>
       <c r="R144" s="10"/>
@@ -21709,7 +21728,7 @@
       </c>
       <c r="I146" s="105"/>
       <c r="J146" s="101" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="K146" s="9" t="s">
         <v>131</v>
@@ -21719,28 +21738,28 @@
       </c>
       <c r="M146" s="168"/>
       <c r="N146" s="10" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="O146" s="102" t="b">
         <f>OR(OR(H138="Fixed Rate Loan",H138="Fixed with embedded Interest Rate Swaps",H138="Fixed without embedded Interest Rate Swaps",H138="Bond / Capital Market product",H138="Development Overdraft", H138="Revolving Loan / Credit Facility",LEFT(H138,8)="Variable",H138="Working Capital Overdraft (if &gt; £1m)"),AND(H138="Fixed Interest Free",H146="Interest Free"))</f>
         <v>0</v>
       </c>
       <c r="P146" s="10" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="Q146" s="102" t="b">
         <f>OR(OR(H146="Base",H146="Interest Free",H146="Lenders Mortgage Base Rate",LEFT(H146,5)="LIBOR",H146="Rate paid by on lender (for on lending only)",H146="RPI linked"),AND(H146="Fixed Rate Percentage",H138="Fixed Rate Loan"))</f>
         <v>0</v>
       </c>
       <c r="R146" s="10" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="S146" s="102" t="b">
         <f>OR(OR(H146="Base",H146="Fixed Rate Percentage",H146="Lenders Mortgage Base Rate",LEFT(H146,5)="LIBOR",H146="Rate paid by on lender (for on lending only)",H146="RPI linked"),AND(H146=" Interest Free",H138="Fixed Interest Free"))</f>
         <v>0</v>
       </c>
       <c r="T146" s="10" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="U146" s="102"/>
       <c r="V146" s="10"/>
@@ -21762,7 +21781,7 @@
         <v>Loan.LPL010</v>
       </c>
       <c r="D147" s="16" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="E147" s="9" t="s">
         <v>1304</v>
@@ -21783,7 +21802,7 @@
         <v>1</v>
       </c>
       <c r="N147" s="10" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="O147" s="102"/>
       <c r="P147" s="10"/>
@@ -21802,14 +21821,14 @@
     </row>
     <row r="148" spans="2:27" ht="116.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B148" s="23" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="C148" s="119" t="str">
         <f t="shared" si="8"/>
         <v>Loan.LPL010a</v>
       </c>
       <c r="D148" s="16" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="E148" s="9" t="s">
         <v>1304</v>
@@ -21830,7 +21849,7 @@
         <v>0</v>
       </c>
       <c r="N148" s="10" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="O148" s="102"/>
       <c r="P148" s="10"/>
@@ -21859,7 +21878,7 @@
         <v>384</v>
       </c>
       <c r="E149" s="23" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="F149" s="17"/>
       <c r="G149" s="17"/>
@@ -21874,7 +21893,7 @@
       <c r="L149" s="10"/>
       <c r="M149" s="102"/>
       <c r="N149" s="10" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="O149" s="102"/>
       <c r="P149" s="10"/>
@@ -21921,14 +21940,14 @@
         <v>1</v>
       </c>
       <c r="N150" s="10" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="O150" s="123" t="b">
         <f>AND(ABS(H150-I13)&lt;=H202,ABS(I13-H150)&lt;=H202)</f>
         <v>0</v>
       </c>
       <c r="P150" s="10" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="Q150" s="102"/>
       <c r="R150" s="144"/>
@@ -21977,14 +21996,14 @@
         <v>1</v>
       </c>
       <c r="N151" s="10" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="O151" s="123" t="b">
         <f>AND(ABS(JH151-I13)&lt;=H203,ABS(I13-H151)&lt;=H202)</f>
         <v>0</v>
       </c>
       <c r="P151" s="10" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="Q151" s="102"/>
       <c r="R151" s="10"/>
@@ -22031,35 +22050,35 @@
         <v>1</v>
       </c>
       <c r="N152" s="10" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="O152" s="102" t="b">
         <f>H152&lt;=H151</f>
         <v>1</v>
       </c>
       <c r="P152" s="10" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="Q152" s="102" t="b">
         <f>OR(OR(H145="Interest only - Bullet repayment at end of term from cashflow",H145="Interest only - Bullet repayment at end of term from refinancing",H145="Interest only then capital and interest",H145="Interest only until fully drawn",H145="Interest only followed by structured capital repayments",H145="Repayable on demand",H145="Converted to loan",H145="Subject to annual renewal"),AND(OR(H145="Fully Amortising",H145="Payment start date deferred then fully amortising", H145="Payment start date deferred-bullet repayment of interest and capital at maturity",H145="Interest &amp; capital then bullet repayment from cashflow or refinancing"),H152=H150))</f>
         <v>0</v>
       </c>
       <c r="R152" s="10" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="S152" s="102" t="b">
         <f>OR(OR(H145="Fully Amortising",H145="Payment start date deferred then fully amortising", H145="Payment start date deferred-bullet repayment of interest and capital at maturity",H145="Interest &amp; capital then bullet repayment from cashflow or refinancing",H145="Interest only - Bullet repayment at end of term from cashflow",H145="Interest only - Bullet repayment at end of term from refinancing", H145="Repayable on demand",H145="Converted to loan",H145="Subject to annual renewal"),AND(OR(H145="Interest only then capital and interest",H145="Interest only until fully drawn",H145="Interest only followed by structured capital repayments",),J152&lt;J150))</f>
         <v>1</v>
       </c>
       <c r="T152" s="10" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="U152" s="102" t="b">
         <f>OR(OR(H145="Fully Amortising",H145="Payment start date deferred then fully amortising", H145="Payment start date deferred-bullet repayment of interest and capital at maturity",H145="Interest &amp; capital then bullet repayment from cashflow or refinancing", H145="Interest only then capital and interest", H145="Interest only followed by structured capital repayments",H145="Repayable on demand",H145="Converted to loan",H145="Subject to annual renewal"),AND(OR(H145="Interest only - Bullet repayment at end of term from cashflow",H145="Interest only - Bullet repayment at end of term from refinancing",H145="Interest only until fully drawn",),L152&lt;L151))</f>
         <v>1</v>
       </c>
       <c r="V152" s="10" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="W152" s="10"/>
       <c r="X152" s="10"/>
@@ -22146,14 +22165,14 @@
         <v>1</v>
       </c>
       <c r="N154" s="10" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="O154" s="102" t="b">
         <f>H154&gt;=I13</f>
         <v>1</v>
       </c>
       <c r="P154" s="10" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="Q154" s="102"/>
       <c r="R154" s="62"/>
@@ -22228,7 +22247,7 @@
         <v>972</v>
       </c>
       <c r="E156" s="23" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="F156" s="17"/>
       <c r="G156" s="17"/>
@@ -22271,10 +22290,10 @@
         <v>Loan.LPL019</v>
       </c>
       <c r="D157" s="16" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="E157" s="23" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="F157" s="17"/>
       <c r="G157" s="17"/>
@@ -22318,7 +22337,7 @@
         <v>338</v>
       </c>
       <c r="E158" s="23" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="F158" s="17"/>
       <c r="G158" s="17"/>
@@ -22362,7 +22381,7 @@
         <v>171</v>
       </c>
       <c r="E159" s="23" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="F159" s="17"/>
       <c r="G159" s="17"/>
@@ -22403,7 +22422,7 @@
         <v>Loan.LPL022</v>
       </c>
       <c r="D160" s="16" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="E160" s="23" t="s">
         <v>134</v>
@@ -22411,7 +22430,7 @@
       <c r="F160" s="17"/>
       <c r="G160" s="17"/>
       <c r="H160" s="104" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="I160" s="105"/>
       <c r="J160" s="101"/>
@@ -22421,7 +22440,7 @@
       <c r="L160" s="10"/>
       <c r="M160" s="102"/>
       <c r="N160" s="10" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="O160" s="102"/>
       <c r="P160" s="10"/>
@@ -22475,7 +22494,7 @@
         <v>1</v>
       </c>
       <c r="N161" s="10" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="O161" s="102"/>
       <c r="P161" s="10"/>
@@ -22501,7 +22520,7 @@
         <v>Loan.LPL024</v>
       </c>
       <c r="D162" s="16" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="E162" s="9" t="s">
         <v>1299</v>
@@ -22522,7 +22541,7 @@
         <v>1</v>
       </c>
       <c r="N162" s="16" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="O162" s="102"/>
       <c r="P162" s="10"/>
@@ -22548,10 +22567,10 @@
         <v>Loan.LPL025</v>
       </c>
       <c r="D163" s="16" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="E163" s="23" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="F163" s="17"/>
       <c r="G163" s="17"/>
@@ -22592,7 +22611,7 @@
         <v>Loan.LPL026</v>
       </c>
       <c r="D164" s="16" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="E164" s="23" t="s">
         <v>130</v>
@@ -22613,14 +22632,14 @@
         <v>0</v>
       </c>
       <c r="N164" s="10" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="O164" s="123" t="b">
         <f>AND(ABS(JH164-I27)&lt;=H202,ABS(I13-H164)&lt;=H202)</f>
         <v>0</v>
       </c>
       <c r="P164" s="10" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="Q164" s="102"/>
       <c r="R164" s="10"/>
@@ -22649,7 +22668,7 @@
         <v>1004</v>
       </c>
       <c r="E165" s="23" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="F165" s="17"/>
       <c r="G165" s="17"/>
@@ -22658,7 +22677,7 @@
       </c>
       <c r="I165" s="105"/>
       <c r="J165" s="120" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="K165" s="9" t="s">
         <v>133</v>
@@ -22686,17 +22705,17 @@
     <row r="166" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="15"/>
       <c r="B166" s="179" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="C166" s="119" t="str">
         <f t="shared" si="8"/>
         <v>Loan.LPL100</v>
       </c>
       <c r="D166" s="180" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E166" s="181" t="s">
         <v>1600</v>
-      </c>
-      <c r="E166" s="181" t="s">
-        <v>1601</v>
       </c>
       <c r="F166" s="183"/>
       <c r="G166" s="183"/>
@@ -22723,17 +22742,17 @@
     <row r="167" spans="1:27" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="15"/>
       <c r="B167" s="179" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="C167" s="119" t="str">
         <f t="shared" si="8"/>
         <v>Loan.LPL101</v>
       </c>
       <c r="D167" s="180" t="s">
+        <v>1604</v>
+      </c>
+      <c r="E167" s="181" t="s">
         <v>1605</v>
-      </c>
-      <c r="E167" s="181" t="s">
-        <v>1606</v>
       </c>
       <c r="F167" s="183"/>
       <c r="G167" s="183"/>
@@ -22767,7 +22786,7 @@
         <v>LoanCovenant.LPC001</v>
       </c>
       <c r="D168" s="109" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="E168" s="108" t="s">
         <v>137</v>
@@ -22776,7 +22795,7 @@
         <v>1262</v>
       </c>
       <c r="G168" s="109" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="H168" s="103"/>
       <c r="I168" s="120" t="e">
@@ -22814,7 +22833,7 @@
         <v>LoanCovenant.LPC002</v>
       </c>
       <c r="D169" s="109" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="E169" s="108" t="s">
         <v>137</v>
@@ -22823,7 +22842,7 @@
         <v>1262</v>
       </c>
       <c r="G169" s="109" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="H169" s="103"/>
       <c r="I169" s="120" t="str">
@@ -22861,7 +22880,7 @@
         <v>LoanCovenant.LPC003</v>
       </c>
       <c r="D170" s="109" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="E170" s="108" t="s">
         <v>1271</v>
@@ -22870,7 +22889,7 @@
         <v>1262</v>
       </c>
       <c r="G170" s="109" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="H170" s="103"/>
       <c r="I170" s="107">
@@ -22912,7 +22931,7 @@
         <v>340</v>
       </c>
       <c r="E171" s="23" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="F171" s="17"/>
       <c r="G171" s="17"/>
@@ -22961,7 +22980,7 @@
       <c r="F172" s="17"/>
       <c r="G172" s="17"/>
       <c r="H172" s="104" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="I172" s="105"/>
       <c r="J172" s="120"/>
@@ -22971,7 +22990,7 @@
       <c r="L172" s="10"/>
       <c r="M172" s="102"/>
       <c r="N172" s="10" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="O172" s="102"/>
       <c r="P172" s="10"/>
@@ -23005,7 +23024,7 @@
       <c r="F173" s="17"/>
       <c r="G173" s="17"/>
       <c r="H173" s="149" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="I173" s="105"/>
       <c r="J173" s="120"/>
@@ -23044,7 +23063,7 @@
         <v>342</v>
       </c>
       <c r="E174" s="23" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="F174" s="17"/>
       <c r="G174" s="17"/>
@@ -23137,7 +23156,7 @@
       <c r="F176" s="17"/>
       <c r="G176" s="17"/>
       <c r="H176" s="149" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="I176" s="105"/>
       <c r="J176" s="120"/>
@@ -23204,7 +23223,7 @@
         <v>EIRD.LPC013</v>
       </c>
       <c r="D178" s="109" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="E178" s="108" t="s">
         <v>1271</v>
@@ -23213,7 +23232,7 @@
         <v>1262</v>
       </c>
       <c r="G178" s="109" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="H178" s="103"/>
       <c r="I178" s="107">
@@ -23253,10 +23272,10 @@
         <v>EIRD.LPC014</v>
       </c>
       <c r="D179" s="16" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="E179" s="23" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="F179" s="17"/>
       <c r="G179" s="17"/>
@@ -23341,7 +23360,7 @@
         <v>EIRD.LPC016</v>
       </c>
       <c r="D181" s="16" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="E181" s="23" t="s">
         <v>130</v>
@@ -23386,7 +23405,7 @@
         <v>EIRD.LPC017</v>
       </c>
       <c r="D182" s="16" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="E182" s="23" t="s">
         <v>130</v>
@@ -23407,7 +23426,7 @@
         <v>1</v>
       </c>
       <c r="N182" s="10" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="O182" s="102"/>
       <c r="P182" s="10"/>
@@ -23428,14 +23447,14 @@
     </row>
     <row r="183" spans="1:27" s="18" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B183" s="23" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="C183" s="119" t="str">
         <f t="shared" si="10"/>
         <v>EIRD.LPC018a</v>
       </c>
       <c r="D183" s="16" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="E183" s="9" t="s">
         <v>1304</v>
@@ -23477,7 +23496,7 @@
         <v>EIRD.LPC018b</v>
       </c>
       <c r="D184" s="16" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="E184" s="9" t="s">
         <v>1304</v>
@@ -23512,14 +23531,14 @@
     </row>
     <row r="185" spans="1:27" s="18" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B185" s="23" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="C185" s="119" t="str">
         <f t="shared" si="10"/>
         <v>EIRD.LPC018c</v>
       </c>
       <c r="D185" s="16" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="E185" s="23" t="s">
         <v>392</v>
@@ -23537,7 +23556,7 @@
       <c r="L185" s="10"/>
       <c r="M185" s="102"/>
       <c r="N185" s="10" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="O185" s="102"/>
       <c r="P185" s="10"/>
@@ -23558,7 +23577,7 @@
       <c r="B186" s="125"/>
       <c r="C186" s="125"/>
       <c r="D186" s="125" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="E186" s="125"/>
       <c r="F186" s="125"/>
@@ -23588,10 +23607,10 @@
         <v>397</v>
       </c>
       <c r="C187" s="64" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="D187" s="126" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="E187" s="23" t="s">
         <v>130</v>
@@ -23614,7 +23633,7 @@
         <v>1</v>
       </c>
       <c r="N187" s="10" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="O187" s="102"/>
       <c r="P187" s="10"/>
@@ -23636,10 +23655,10 @@
         <v>398</v>
       </c>
       <c r="C188" s="64" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D188" s="126" t="s">
         <v>1406</v>
-      </c>
-      <c r="D188" s="126" t="s">
-        <v>1407</v>
       </c>
       <c r="E188" s="23" t="s">
         <v>138</v>
@@ -23647,7 +23666,7 @@
       <c r="F188" s="17"/>
       <c r="G188" s="17"/>
       <c r="H188" s="100" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="I188" s="100"/>
       <c r="J188" s="105"/>
@@ -23679,7 +23698,7 @@
         <v>399</v>
       </c>
       <c r="C189" s="64" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="D189" s="126" t="s">
         <v>396</v>
@@ -23690,7 +23709,7 @@
       <c r="F189" s="23"/>
       <c r="G189" s="23"/>
       <c r="H189" s="100" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="I189" s="100"/>
       <c r="J189" s="105"/>
@@ -23722,13 +23741,13 @@
         <v>399</v>
       </c>
       <c r="C190" s="64" t="s">
+        <v>1583</v>
+      </c>
+      <c r="D190" s="126" t="s">
         <v>1584</v>
       </c>
-      <c r="D190" s="126" t="s">
+      <c r="E190" s="23" t="s">
         <v>1585</v>
-      </c>
-      <c r="E190" s="23" t="s">
-        <v>1586</v>
       </c>
       <c r="F190" s="23"/>
       <c r="G190" s="23"/>
@@ -23756,7 +23775,7 @@
       <c r="B191" s="127"/>
       <c r="C191" s="24"/>
       <c r="D191" s="19" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="E191" s="12"/>
       <c r="F191" s="12"/>
@@ -23781,23 +23800,23 @@
     </row>
     <row r="192" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B192" s="129" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="C192" s="130" t="s">
+        <v>1411</v>
+      </c>
+      <c r="D192" s="130" t="s">
         <v>1412</v>
       </c>
-      <c r="D192" s="130" t="s">
+      <c r="E192" s="129" t="s">
         <v>1413</v>
       </c>
-      <c r="E192" s="129" t="s">
+      <c r="F192" s="129" t="s">
         <v>1414</v>
-      </c>
-      <c r="F192" s="129" t="s">
-        <v>1415</v>
       </c>
       <c r="G192" s="130"/>
       <c r="H192" s="101" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="I192" s="101"/>
       <c r="J192" s="101"/>
@@ -23820,23 +23839,23 @@
     </row>
     <row r="193" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B193" s="129" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="C193" s="130" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D193" s="130" t="s">
         <v>1417</v>
       </c>
-      <c r="D193" s="130" t="s">
+      <c r="E193" s="129" t="s">
         <v>1418</v>
-      </c>
-      <c r="E193" s="129" t="s">
-        <v>1419</v>
       </c>
       <c r="F193" s="129" t="s">
         <v>1262</v>
       </c>
       <c r="G193" s="130"/>
       <c r="H193" s="101" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="I193" s="101"/>
       <c r="J193" s="101"/>
@@ -23859,16 +23878,16 @@
     </row>
     <row r="194" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B194" s="129" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="C194" s="130" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D194" s="130" t="s">
         <v>1025</v>
       </c>
       <c r="E194" s="129" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="F194" s="129" t="s">
         <v>1262</v>
@@ -23898,19 +23917,19 @@
     </row>
     <row r="195" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B195" s="129" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="C195" s="130" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D195" s="130" t="s">
         <v>1422</v>
       </c>
-      <c r="D195" s="130" t="s">
+      <c r="E195" s="129" t="s">
         <v>1423</v>
       </c>
-      <c r="E195" s="129" t="s">
-        <v>1424</v>
-      </c>
       <c r="F195" s="129" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="G195" s="130"/>
       <c r="H195" s="121">
@@ -23937,19 +23956,19 @@
     </row>
     <row r="196" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B196" s="129" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="C196" s="130" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D196" s="130" t="s">
         <v>1425</v>
       </c>
-      <c r="D196" s="130" t="s">
-        <v>1426</v>
-      </c>
       <c r="E196" s="129" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F196" s="129" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="G196" s="130"/>
       <c r="H196" s="121">
@@ -23976,23 +23995,23 @@
     </row>
     <row r="197" spans="2:24" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B197" s="129" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="C197" s="130" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D197" s="130" t="s">
         <v>1427</v>
       </c>
-      <c r="D197" s="130" t="s">
+      <c r="E197" s="129" t="s">
         <v>1428</v>
       </c>
-      <c r="E197" s="129" t="s">
-        <v>1429</v>
-      </c>
       <c r="F197" s="129" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="G197" s="130"/>
       <c r="H197" s="101" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="I197" s="101"/>
       <c r="J197" s="101"/>
@@ -24015,19 +24034,19 @@
     </row>
     <row r="198" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B198" s="129" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="C198" s="130" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D198" s="130" t="s">
         <v>1431</v>
       </c>
-      <c r="D198" s="130" t="s">
+      <c r="E198" s="129" t="s">
         <v>1432</v>
       </c>
-      <c r="E198" s="129" t="s">
-        <v>1433</v>
-      </c>
       <c r="F198" s="129" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="G198" s="130"/>
       <c r="H198" s="99">
@@ -24054,19 +24073,19 @@
     </row>
     <row r="199" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B199" s="129" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="C199" s="130" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D199" s="130" t="s">
         <v>1434</v>
       </c>
-      <c r="D199" s="130" t="s">
-        <v>1435</v>
-      </c>
       <c r="E199" s="129" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="F199" s="129" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="G199" s="130"/>
       <c r="H199" s="99">
@@ -24093,19 +24112,19 @@
     </row>
     <row r="200" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B200" s="129" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="C200" s="130" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D200" s="130" t="s">
         <v>1436</v>
       </c>
-      <c r="D200" s="130" t="s">
-        <v>1437</v>
-      </c>
       <c r="E200" s="129" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="F200" s="129" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="G200" s="130"/>
       <c r="H200" s="99">
@@ -24132,19 +24151,19 @@
     </row>
     <row r="201" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B201" s="129" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C201" s="130" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="D201" s="130" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="E201" s="129" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="F201" s="129" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="G201" s="130"/>
       <c r="H201" s="99">
@@ -24171,19 +24190,19 @@
     </row>
     <row r="202" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B202" s="129" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="C202" s="130" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D202" s="130" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="E202" s="129" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="F202" s="129" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="G202" s="130"/>
       <c r="H202" s="99">
@@ -24209,21 +24228,21 @@
     </row>
     <row r="203" spans="2:24" ht="318.75" x14ac:dyDescent="0.2">
       <c r="B203" s="129" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="C203" s="130" t="s">
+        <v>1441</v>
+      </c>
+      <c r="D203" s="130" t="s">
         <v>1442</v>
       </c>
-      <c r="D203" s="130" t="s">
+      <c r="E203" s="129" t="s">
         <v>1443</v>
-      </c>
-      <c r="E203" s="129" t="s">
-        <v>1444</v>
       </c>
       <c r="F203" s="129"/>
       <c r="G203" s="130"/>
       <c r="H203" s="121" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="I203" s="121"/>
       <c r="J203" s="101"/>
@@ -24244,21 +24263,21 @@
     </row>
     <row r="204" spans="2:24" ht="409.5" x14ac:dyDescent="0.2">
       <c r="B204" s="129" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="C204" s="130" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D204" s="130" t="s">
         <v>1446</v>
       </c>
-      <c r="D204" s="130" t="s">
-        <v>1447</v>
-      </c>
       <c r="E204" s="129" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F204" s="129"/>
       <c r="G204" s="130"/>
       <c r="H204" s="121" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="I204" s="121"/>
       <c r="J204" s="101"/>
@@ -24279,21 +24298,21 @@
     </row>
     <row r="205" spans="2:24" ht="357" x14ac:dyDescent="0.2">
       <c r="B205" s="129" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="C205" s="130" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D205" s="130" t="s">
         <v>1448</v>
       </c>
-      <c r="D205" s="130" t="s">
-        <v>1449</v>
-      </c>
       <c r="E205" s="129" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F205" s="129"/>
       <c r="G205" s="130"/>
       <c r="H205" s="121" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="I205" s="121"/>
       <c r="J205" s="101"/>
@@ -24314,21 +24333,21 @@
     </row>
     <row r="206" spans="2:24" ht="229.5" x14ac:dyDescent="0.2">
       <c r="B206" s="129" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="C206" s="130" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D206" s="130" t="s">
         <v>1451</v>
       </c>
-      <c r="D206" s="130" t="s">
-        <v>1452</v>
-      </c>
       <c r="E206" s="129" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F206" s="129"/>
       <c r="G206" s="130"/>
       <c r="H206" s="101" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="I206" s="101"/>
       <c r="J206" s="101"/>
@@ -24349,21 +24368,21 @@
     </row>
     <row r="207" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B207" s="167" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="C207" s="207" t="s">
+        <v>1609</v>
+      </c>
+      <c r="D207" s="207" t="s">
         <v>1610</v>
       </c>
-      <c r="D207" s="207" t="s">
-        <v>1611</v>
-      </c>
       <c r="E207" s="129" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="F207" s="166"/>
       <c r="G207" s="207"/>
       <c r="H207" s="208" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="I207" s="208"/>
       <c r="J207" s="208"/>
@@ -24384,16 +24403,16 @@
     </row>
     <row r="208" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B208" s="167" t="s">
+        <v>1628</v>
+      </c>
+      <c r="C208" s="207" t="s">
         <v>1629</v>
       </c>
-      <c r="C208" s="207" t="s">
+      <c r="D208" s="207" t="s">
         <v>1630</v>
       </c>
-      <c r="D208" s="207" t="s">
-        <v>1631</v>
-      </c>
       <c r="E208" s="166" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F208" s="166"/>
       <c r="G208" s="207"/>
@@ -24419,16 +24438,16 @@
     </row>
     <row r="209" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B209" s="167" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="C209" s="207" t="s">
+        <v>1631</v>
+      </c>
+      <c r="D209" s="207" t="s">
         <v>1632</v>
       </c>
-      <c r="D209" s="207" t="s">
-        <v>1633</v>
-      </c>
       <c r="E209" s="166" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F209" s="166"/>
       <c r="G209" s="207"/>
@@ -24454,7 +24473,7 @@
     </row>
     <row r="210" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B210" s="167" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
   </sheetData>
@@ -24564,7 +24583,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="B10" t="str">
         <f>Data!H11</f>
@@ -24670,13 +24689,13 @@
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="135"/>
       <c r="B32" s="136" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="44"/>
       <c r="B34" s="44" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -24719,7 +24738,7 @@
         <v>10000</v>
       </c>
       <c r="E36" s="142" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="F36" s="112">
         <f>Data!H37</f>
@@ -24748,7 +24767,7 @@
         <v>Borrow</v>
       </c>
       <c r="D37" s="142" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="E37" s="141">
         <f>Data!H62</f>
@@ -24776,7 +24795,7 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="44"/>
       <c r="B39" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -24837,7 +24856,7 @@
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="44"/>
       <c r="B45" s="33" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -24926,7 +24945,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B52" s="33" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
   </sheetData>
@@ -25031,9 +25050,9 @@
       <c r="A22" s="44" t="s">
         <v>190</v>
       </c>
-      <c r="B22" t="str">
+      <c r="B22">
         <f>Data!H34</f>
-        <v>Capital Purchase (give details)</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -25135,9 +25154,9 @@
       <c r="A42" s="44" t="s">
         <v>197</v>
       </c>
-      <c r="B42" t="str">
+      <c r="B42">
         <f>Data!H44</f>
-        <v>Yes</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -25187,7 +25206,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="44" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B54">
         <f>Data!H50</f>
@@ -25207,9 +25226,9 @@
       <c r="A58" s="44" t="s">
         <v>1291</v>
       </c>
-      <c r="B58" t="str">
+      <c r="B58">
         <f>Data!H52</f>
-        <v>Yes</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -25260,7 +25279,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -25485,7 +25504,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="44" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B54">
         <f>Data!H80</f>
@@ -25503,7 +25522,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="44" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="B58" t="b">
         <f>Data!H82</f>
@@ -25538,7 +25557,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -25600,7 +25619,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="44" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="B22">
         <f>Data!H91</f>
@@ -25609,7 +25628,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="44" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="B24">
         <f>Data!H92</f>
@@ -25704,7 +25723,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B42" s="44" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -25743,7 +25762,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
   </sheetData>
@@ -25778,7 +25797,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="B3" s="140">
         <f>Data!I103</f>
@@ -25787,7 +25806,7 @@
     </row>
     <row r="5" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="44" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B5" s="140">
         <f>Data!I104</f>
@@ -25874,7 +25893,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="44" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -25882,7 +25901,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="B10" t="str">
         <f>Data!H113</f>
@@ -25909,7 +25928,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="44" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="B16" s="145" t="str">
         <f>Data!I116</f>
@@ -25918,7 +25937,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="44" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="B18" s="141" t="str">
         <f>Data!H117</f>
@@ -26022,7 +26041,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="44" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B38" s="112" t="str">
         <f>Data!H127</f>
@@ -26040,7 +26059,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="146" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -26048,7 +26067,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="44" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="B44" t="b">
         <f>Data!H129</f>
@@ -26075,7 +26094,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="44" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="B50" t="str">
         <f>Data!H132</f>
@@ -26084,7 +26103,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="44" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="B52" t="b">
         <f>Data!H133</f>
@@ -26093,7 +26112,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B54" s="44" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>

</xml_diff>